<commit_message>
Changed all files for new forms after long time
</commit_message>
<xml_diff>
--- a/Excell/zhr_zam.xlsx
+++ b/Excell/zhr_zam.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B21267-F5E8-41EF-B3E7-8ABFD283C1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="38280" yWindow="1095" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,9 +28,6 @@
     <t>Дата записи</t>
   </si>
   <si>
-    <t>Содержание замечания и предложения (выявленные отступления от проектно-сметной документации, нарушения СНиП и т.д.)</t>
-  </si>
-  <si>
     <t>Запись произвел (должность, организация, Ф.И.О. контролирующего лица)</t>
   </si>
   <si>
@@ -37,9 +35,6 @@
   </si>
   <si>
     <t>Сведения об устранении замечаний</t>
-  </si>
-  <si>
-    <t>Ф.И.О., должность, подпись ответственного лица, проверяющего журнал</t>
   </si>
   <si>
     <t>Работы закончены. Журнал закрыт.</t>
@@ -106,11 +101,21 @@
   <si>
     <t>ЖУРНАЛ №1</t>
   </si>
+  <si>
+    <t>Содержание замечаний и предложений
+(выявленные отступления от проектной и рабочей документации, нарушения
+требований строительных норм и правил
+по производству строительно- монтажных работ и т.д.)</t>
+  </si>
+  <si>
+    <t>Инициалы, фамилия, должность и подпись ответственного лица,
+проверя_x0002_ющего журнал</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,6 +397,51 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -407,51 +457,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -461,6 +466,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -509,7 +517,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,9 +550,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -577,6 +602,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -752,17 +794,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT182"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM1:AM1048576"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="BA36" sqref="BA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="15" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3" customWidth="1"/>
+    <col min="4" max="15" width="2.28515625" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="17" max="18" width="2.85546875" customWidth="1"/>
     <col min="19" max="19" width="4" customWidth="1"/>
@@ -773,202 +817,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="21"/>
-      <c r="AS1" s="21"/>
-      <c r="AT1" s="21"/>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
     </row>
     <row r="3" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21"/>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
-      <c r="AP3" s="21"/>
-      <c r="AQ3" s="21"/>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="21"/>
-      <c r="AT3" s="21"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="36"/>
+      <c r="AE3" s="36"/>
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" s="36"/>
+      <c r="AJ3" s="36"/>
+      <c r="AK3" s="36"/>
+      <c r="AL3" s="36"/>
+      <c r="AM3" s="36"/>
+      <c r="AN3" s="36"/>
+      <c r="AO3" s="36"/>
+      <c r="AP3" s="36"/>
+      <c r="AQ3" s="36"/>
+      <c r="AR3" s="36"/>
+      <c r="AS3" s="36"/>
+      <c r="AT3" s="36"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>13</v>
+      <c r="A4" s="37" t="s">
+        <v>11</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="22"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="22"/>
-      <c r="AQ4" s="22"/>
-      <c r="AR4" s="22"/>
-      <c r="AS4" s="22"/>
-      <c r="AT4" s="22"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37"/>
+      <c r="AN4" s="37"/>
+      <c r="AO4" s="37"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="37"/>
+      <c r="AR4" s="37"/>
+      <c r="AS4" s="37"/>
+      <c r="AT4" s="37"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -1259,104 +1303,104 @@
       <c r="AT10" s="3"/>
     </row>
     <row r="11" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>20</v>
+      <c r="A11" s="38" t="s">
+        <v>18</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
-      <c r="AI11" s="23"/>
-      <c r="AJ11" s="23"/>
-      <c r="AK11" s="23"/>
-      <c r="AL11" s="23"/>
-      <c r="AM11" s="23"/>
-      <c r="AN11" s="23"/>
-      <c r="AO11" s="23"/>
-      <c r="AP11" s="23"/>
-      <c r="AQ11" s="23"/>
-      <c r="AR11" s="23"/>
-      <c r="AS11" s="23"/>
-      <c r="AT11" s="23"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="38"/>
+      <c r="AI11" s="38"/>
+      <c r="AJ11" s="38"/>
+      <c r="AK11" s="38"/>
+      <c r="AL11" s="38"/>
+      <c r="AM11" s="38"/>
+      <c r="AN11" s="38"/>
+      <c r="AO11" s="38"/>
+      <c r="AP11" s="38"/>
+      <c r="AQ11" s="38"/>
+      <c r="AR11" s="38"/>
+      <c r="AS11" s="38"/>
+      <c r="AT11" s="38"/>
     </row>
     <row r="12" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>15</v>
+      <c r="A12" s="38" t="s">
+        <v>13</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="23"/>
-      <c r="AE12" s="23"/>
-      <c r="AF12" s="23"/>
-      <c r="AG12" s="23"/>
-      <c r="AH12" s="23"/>
-      <c r="AI12" s="23"/>
-      <c r="AJ12" s="23"/>
-      <c r="AK12" s="23"/>
-      <c r="AL12" s="23"/>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="23"/>
-      <c r="AP12" s="23"/>
-      <c r="AQ12" s="23"/>
-      <c r="AR12" s="23"/>
-      <c r="AS12" s="23"/>
-      <c r="AT12" s="23"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="38"/>
+      <c r="AC12" s="38"/>
+      <c r="AD12" s="38"/>
+      <c r="AE12" s="38"/>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="38"/>
+      <c r="AI12" s="38"/>
+      <c r="AJ12" s="38"/>
+      <c r="AK12" s="38"/>
+      <c r="AL12" s="38"/>
+      <c r="AM12" s="38"/>
+      <c r="AN12" s="38"/>
+      <c r="AO12" s="38"/>
+      <c r="AP12" s="38"/>
+      <c r="AQ12" s="38"/>
+      <c r="AR12" s="38"/>
+      <c r="AS12" s="38"/>
+      <c r="AT12" s="38"/>
     </row>
     <row r="13" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
@@ -1456,7 +1500,7 @@
     </row>
     <row r="15" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -1506,7 +1550,7 @@
     </row>
     <row r="16" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1519,40 +1563,40 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="24"/>
-      <c r="AE16" s="24"/>
-      <c r="AF16" s="24"/>
-      <c r="AG16" s="24"/>
-      <c r="AH16" s="24"/>
-      <c r="AI16" s="24"/>
-      <c r="AJ16" s="24"/>
-      <c r="AK16" s="24"/>
-      <c r="AL16" s="24"/>
-      <c r="AM16" s="24"/>
-      <c r="AN16" s="24"/>
-      <c r="AO16" s="24"/>
-      <c r="AP16" s="24"/>
-      <c r="AQ16" s="24"/>
-      <c r="AR16" s="24"/>
-      <c r="AS16" s="24"/>
-      <c r="AT16" s="24"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="39"/>
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="39"/>
+      <c r="AG16" s="39"/>
+      <c r="AH16" s="39"/>
+      <c r="AI16" s="39"/>
+      <c r="AJ16" s="39"/>
+      <c r="AK16" s="39"/>
+      <c r="AL16" s="39"/>
+      <c r="AM16" s="39"/>
+      <c r="AN16" s="39"/>
+      <c r="AO16" s="39"/>
+      <c r="AP16" s="39"/>
+      <c r="AQ16" s="39"/>
+      <c r="AR16" s="39"/>
+      <c r="AS16" s="39"/>
+      <c r="AT16" s="39"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1567,42 +1611,42 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="20" t="s">
-        <v>18</v>
+      <c r="M17" s="35" t="s">
+        <v>16</v>
       </c>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
-      <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20"/>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
-      <c r="AG17" s="20"/>
-      <c r="AH17" s="20"/>
-      <c r="AI17" s="20"/>
-      <c r="AJ17" s="20"/>
-      <c r="AK17" s="20"/>
-      <c r="AL17" s="20"/>
-      <c r="AM17" s="20"/>
-      <c r="AN17" s="20"/>
-      <c r="AO17" s="20"/>
-      <c r="AP17" s="20"/>
-      <c r="AQ17" s="20"/>
-      <c r="AR17" s="20"/>
-      <c r="AS17" s="20"/>
-      <c r="AT17" s="20"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="35"/>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="35"/>
+      <c r="AC17" s="35"/>
+      <c r="AD17" s="35"/>
+      <c r="AE17" s="35"/>
+      <c r="AF17" s="35"/>
+      <c r="AG17" s="35"/>
+      <c r="AH17" s="35"/>
+      <c r="AI17" s="35"/>
+      <c r="AJ17" s="35"/>
+      <c r="AK17" s="35"/>
+      <c r="AL17" s="35"/>
+      <c r="AM17" s="35"/>
+      <c r="AN17" s="35"/>
+      <c r="AO17" s="35"/>
+      <c r="AP17" s="35"/>
+      <c r="AQ17" s="35"/>
+      <c r="AR17" s="35"/>
+      <c r="AS17" s="35"/>
+      <c r="AT17" s="35"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -1654,7 +1698,7 @@
     </row>
     <row r="19" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1704,7 +1748,7 @@
     </row>
     <row r="20" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1717,40 +1761,40 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
-      <c r="AG20" s="24"/>
-      <c r="AH20" s="24"/>
-      <c r="AI20" s="24"/>
-      <c r="AJ20" s="24"/>
-      <c r="AK20" s="24"/>
-      <c r="AL20" s="24"/>
-      <c r="AM20" s="24"/>
-      <c r="AN20" s="24"/>
-      <c r="AO20" s="24"/>
-      <c r="AP20" s="24"/>
-      <c r="AQ20" s="24"/>
-      <c r="AR20" s="24"/>
-      <c r="AS20" s="24"/>
-      <c r="AT20" s="24"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="39"/>
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="39"/>
+      <c r="AG20" s="39"/>
+      <c r="AH20" s="39"/>
+      <c r="AI20" s="39"/>
+      <c r="AJ20" s="39"/>
+      <c r="AK20" s="39"/>
+      <c r="AL20" s="39"/>
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="39"/>
+      <c r="AO20" s="39"/>
+      <c r="AP20" s="39"/>
+      <c r="AQ20" s="39"/>
+      <c r="AR20" s="39"/>
+      <c r="AS20" s="39"/>
+      <c r="AT20" s="39"/>
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1765,42 +1809,42 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="20" t="s">
-        <v>18</v>
+      <c r="M21" s="35" t="s">
+        <v>16</v>
       </c>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="20"/>
-      <c r="W21" s="20"/>
-      <c r="X21" s="20"/>
-      <c r="Y21" s="20"/>
-      <c r="Z21" s="20"/>
-      <c r="AA21" s="20"/>
-      <c r="AB21" s="20"/>
-      <c r="AC21" s="20"/>
-      <c r="AD21" s="20"/>
-      <c r="AE21" s="20"/>
-      <c r="AF21" s="20"/>
-      <c r="AG21" s="20"/>
-      <c r="AH21" s="20"/>
-      <c r="AI21" s="20"/>
-      <c r="AJ21" s="20"/>
-      <c r="AK21" s="20"/>
-      <c r="AL21" s="20"/>
-      <c r="AM21" s="20"/>
-      <c r="AN21" s="20"/>
-      <c r="AO21" s="20"/>
-      <c r="AP21" s="20"/>
-      <c r="AQ21" s="20"/>
-      <c r="AR21" s="20"/>
-      <c r="AS21" s="20"/>
-      <c r="AT21" s="20"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="35"/>
+      <c r="Z21" s="35"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="35"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="35"/>
+      <c r="AE21" s="35"/>
+      <c r="AF21" s="35"/>
+      <c r="AG21" s="35"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="35"/>
+      <c r="AJ21" s="35"/>
+      <c r="AK21" s="35"/>
+      <c r="AL21" s="35"/>
+      <c r="AM21" s="35"/>
+      <c r="AN21" s="35"/>
+      <c r="AO21" s="35"/>
+      <c r="AP21" s="35"/>
+      <c r="AQ21" s="35"/>
+      <c r="AR21" s="35"/>
+      <c r="AS21" s="35"/>
+      <c r="AT21" s="35"/>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -2081,7 +2125,7 @@
       <c r="AJ27" s="5"/>
       <c r="AK27" s="2"/>
       <c r="AL27" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AM27" s="4" t="s">
         <v>0</v>
@@ -2181,7 +2225,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
       <c r="AL29" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AM29" s="4" t="s">
         <v>0</v>
@@ -2242,1713 +2286,1713 @@
       <c r="AS33" s="6"/>
       <c r="AT33" s="6"/>
     </row>
-    <row r="34" spans="1:46" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="29" t="s">
+    <row r="34" spans="1:46" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q34" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
+      <c r="T34" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="28" t="s">
-        <v>9</v>
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
+      <c r="W34" s="34"/>
+      <c r="X34" s="34"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="34"/>
+      <c r="AA34" s="34" t="s">
+        <v>3</v>
       </c>
-      <c r="Q34" s="28" t="s">
+      <c r="AB34" s="34"/>
+      <c r="AC34" s="34"/>
+      <c r="AD34" s="34"/>
+      <c r="AE34" s="34"/>
+      <c r="AF34" s="34"/>
+      <c r="AG34" s="34"/>
+      <c r="AH34" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI34" s="34"/>
+      <c r="AJ34" s="34"/>
+      <c r="AK34" s="34"/>
+      <c r="AL34" s="34"/>
+      <c r="AM34" s="34"/>
+      <c r="AN34" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO34" s="34"/>
+      <c r="AP34" s="34"/>
+      <c r="AQ34" s="34"/>
+      <c r="AR34" s="34"/>
+      <c r="AS34" s="34"/>
+      <c r="AT34" s="34"/>
+    </row>
+    <row r="35" spans="1:46" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="34"/>
+      <c r="Q35" s="34"/>
+      <c r="R35" s="34"/>
+      <c r="S35" s="34"/>
+      <c r="T35" s="34"/>
+      <c r="U35" s="34"/>
+      <c r="V35" s="34"/>
+      <c r="W35" s="34"/>
+      <c r="X35" s="34"/>
+      <c r="Y35" s="34"/>
+      <c r="Z35" s="34"/>
+      <c r="AA35" s="34"/>
+      <c r="AB35" s="34"/>
+      <c r="AC35" s="34"/>
+      <c r="AD35" s="34"/>
+      <c r="AE35" s="34"/>
+      <c r="AF35" s="34"/>
+      <c r="AG35" s="34"/>
+      <c r="AH35" s="34"/>
+      <c r="AI35" s="34"/>
+      <c r="AJ35" s="34"/>
+      <c r="AK35" s="34"/>
+      <c r="AL35" s="34"/>
+      <c r="AM35" s="34"/>
+      <c r="AN35" s="34"/>
+      <c r="AO35" s="34"/>
+      <c r="AP35" s="34"/>
+      <c r="AQ35" s="34"/>
+      <c r="AR35" s="34"/>
+      <c r="AS35" s="34"/>
+      <c r="AT35" s="34"/>
+    </row>
+    <row r="36" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="34"/>
+      <c r="U36" s="34"/>
+      <c r="V36" s="34"/>
+      <c r="W36" s="34"/>
+      <c r="X36" s="34"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="34"/>
+      <c r="AA36" s="34"/>
+      <c r="AB36" s="34"/>
+      <c r="AC36" s="34"/>
+      <c r="AD36" s="34"/>
+      <c r="AE36" s="34"/>
+      <c r="AF36" s="34"/>
+      <c r="AG36" s="34"/>
+      <c r="AH36" s="34"/>
+      <c r="AI36" s="34"/>
+      <c r="AJ36" s="34"/>
+      <c r="AK36" s="34"/>
+      <c r="AL36" s="34"/>
+      <c r="AM36" s="34"/>
+      <c r="AN36" s="34"/>
+      <c r="AO36" s="34"/>
+      <c r="AP36" s="34"/>
+      <c r="AQ36" s="34"/>
+      <c r="AR36" s="34"/>
+      <c r="AS36" s="34"/>
+      <c r="AT36" s="34"/>
+    </row>
+    <row r="37" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="34"/>
+      <c r="R37" s="34"/>
+      <c r="S37" s="34"/>
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="34"/>
+      <c r="Y37" s="34"/>
+      <c r="Z37" s="34"/>
+      <c r="AA37" s="34"/>
+      <c r="AB37" s="34"/>
+      <c r="AC37" s="34"/>
+      <c r="AD37" s="34"/>
+      <c r="AE37" s="34"/>
+      <c r="AF37" s="34"/>
+      <c r="AG37" s="34"/>
+      <c r="AH37" s="34"/>
+      <c r="AI37" s="34"/>
+      <c r="AJ37" s="34"/>
+      <c r="AK37" s="34"/>
+      <c r="AL37" s="34"/>
+      <c r="AM37" s="34"/>
+      <c r="AN37" s="34"/>
+      <c r="AO37" s="34"/>
+      <c r="AP37" s="34"/>
+      <c r="AQ37" s="34"/>
+      <c r="AR37" s="34"/>
+      <c r="AS37" s="34"/>
+      <c r="AT37" s="34"/>
+    </row>
+    <row r="38" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="20">
         <v>1</v>
       </c>
-      <c r="R34" s="28"/>
-      <c r="S34" s="28"/>
-      <c r="T34" s="28" t="s">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="15">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="23">
         <v>3</v>
       </c>
-      <c r="U34" s="28"/>
-      <c r="V34" s="28"/>
-      <c r="W34" s="28"/>
-      <c r="X34" s="28"/>
-      <c r="Y34" s="28"/>
-      <c r="Z34" s="28"/>
-      <c r="AA34" s="28" t="s">
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23">
         <v>4</v>
       </c>
-      <c r="AB34" s="28"/>
-      <c r="AC34" s="28"/>
-      <c r="AD34" s="28"/>
-      <c r="AE34" s="28"/>
-      <c r="AF34" s="28"/>
-      <c r="AG34" s="28"/>
-      <c r="AH34" s="28" t="s">
+      <c r="U38" s="23"/>
+      <c r="V38" s="23"/>
+      <c r="W38" s="23"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="23"/>
+      <c r="AA38" s="23">
         <v>5</v>
       </c>
-      <c r="AI34" s="28"/>
-      <c r="AJ34" s="28"/>
-      <c r="AK34" s="28"/>
-      <c r="AL34" s="28"/>
-      <c r="AM34" s="28"/>
-      <c r="AN34" s="28" t="s">
+      <c r="AB38" s="23"/>
+      <c r="AC38" s="23"/>
+      <c r="AD38" s="23"/>
+      <c r="AE38" s="23"/>
+      <c r="AF38" s="23"/>
+      <c r="AG38" s="23"/>
+      <c r="AH38" s="23">
         <v>6</v>
       </c>
-      <c r="AO34" s="28"/>
-      <c r="AP34" s="28"/>
-      <c r="AQ34" s="28"/>
-      <c r="AR34" s="28"/>
-      <c r="AS34" s="28"/>
-      <c r="AT34" s="28"/>
-    </row>
-    <row r="35" spans="1:46" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="28"/>
-      <c r="Q35" s="28"/>
-      <c r="R35" s="28"/>
-      <c r="S35" s="28"/>
-      <c r="T35" s="28"/>
-      <c r="U35" s="28"/>
-      <c r="V35" s="28"/>
-      <c r="W35" s="28"/>
-      <c r="X35" s="28"/>
-      <c r="Y35" s="28"/>
-      <c r="Z35" s="28"/>
-      <c r="AA35" s="28"/>
-      <c r="AB35" s="28"/>
-      <c r="AC35" s="28"/>
-      <c r="AD35" s="28"/>
-      <c r="AE35" s="28"/>
-      <c r="AF35" s="28"/>
-      <c r="AG35" s="28"/>
-      <c r="AH35" s="28"/>
-      <c r="AI35" s="28"/>
-      <c r="AJ35" s="28"/>
-      <c r="AK35" s="28"/>
-      <c r="AL35" s="28"/>
-      <c r="AM35" s="28"/>
-      <c r="AN35" s="28"/>
-      <c r="AO35" s="28"/>
-      <c r="AP35" s="28"/>
-      <c r="AQ35" s="28"/>
-      <c r="AR35" s="28"/>
-      <c r="AS35" s="28"/>
-      <c r="AT35" s="28"/>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="28"/>
-      <c r="Q36" s="28"/>
-      <c r="R36" s="28"/>
-      <c r="S36" s="28"/>
-      <c r="T36" s="28"/>
-      <c r="U36" s="28"/>
-      <c r="V36" s="28"/>
-      <c r="W36" s="28"/>
-      <c r="X36" s="28"/>
-      <c r="Y36" s="28"/>
-      <c r="Z36" s="28"/>
-      <c r="AA36" s="28"/>
-      <c r="AB36" s="28"/>
-      <c r="AC36" s="28"/>
-      <c r="AD36" s="28"/>
-      <c r="AE36" s="28"/>
-      <c r="AF36" s="28"/>
-      <c r="AG36" s="28"/>
-      <c r="AH36" s="28"/>
-      <c r="AI36" s="28"/>
-      <c r="AJ36" s="28"/>
-      <c r="AK36" s="28"/>
-      <c r="AL36" s="28"/>
-      <c r="AM36" s="28"/>
-      <c r="AN36" s="28"/>
-      <c r="AO36" s="28"/>
-      <c r="AP36" s="28"/>
-      <c r="AQ36" s="28"/>
-      <c r="AR36" s="28"/>
-      <c r="AS36" s="28"/>
-      <c r="AT36" s="28"/>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="28"/>
-      <c r="Q37" s="28"/>
-      <c r="R37" s="28"/>
-      <c r="S37" s="28"/>
-      <c r="T37" s="28"/>
-      <c r="U37" s="28"/>
-      <c r="V37" s="28"/>
-      <c r="W37" s="28"/>
-      <c r="X37" s="28"/>
-      <c r="Y37" s="28"/>
-      <c r="Z37" s="28"/>
-      <c r="AA37" s="28"/>
-      <c r="AB37" s="28"/>
-      <c r="AC37" s="28"/>
-      <c r="AD37" s="28"/>
-      <c r="AE37" s="28"/>
-      <c r="AF37" s="28"/>
-      <c r="AG37" s="28"/>
-      <c r="AH37" s="28"/>
-      <c r="AI37" s="28"/>
-      <c r="AJ37" s="28"/>
-      <c r="AK37" s="28"/>
-      <c r="AL37" s="28"/>
-      <c r="AM37" s="28"/>
-      <c r="AN37" s="28"/>
-      <c r="AO37" s="28"/>
-      <c r="AP37" s="28"/>
-      <c r="AQ37" s="28"/>
-      <c r="AR37" s="28"/>
-      <c r="AS37" s="28"/>
-      <c r="AT37" s="28"/>
-    </row>
-    <row r="38" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="26">
-        <v>2</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="15">
-        <v>3</v>
-      </c>
-      <c r="Q38" s="25">
-        <v>4</v>
-      </c>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25">
-        <v>5</v>
-      </c>
-      <c r="U38" s="25"/>
-      <c r="V38" s="25"/>
-      <c r="W38" s="25"/>
-      <c r="X38" s="25"/>
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
-      <c r="AA38" s="25">
-        <v>6</v>
-      </c>
-      <c r="AB38" s="25"/>
-      <c r="AC38" s="25"/>
-      <c r="AD38" s="25"/>
-      <c r="AE38" s="25"/>
-      <c r="AF38" s="25"/>
-      <c r="AG38" s="25"/>
-      <c r="AH38" s="25">
+      <c r="AI38" s="23"/>
+      <c r="AJ38" s="23"/>
+      <c r="AK38" s="23"/>
+      <c r="AL38" s="23"/>
+      <c r="AM38" s="23"/>
+      <c r="AN38" s="23">
         <v>7</v>
       </c>
-      <c r="AI38" s="25"/>
-      <c r="AJ38" s="25"/>
-      <c r="AK38" s="25"/>
-      <c r="AL38" s="25"/>
-      <c r="AM38" s="25"/>
-      <c r="AN38" s="25">
-        <v>8</v>
-      </c>
-      <c r="AO38" s="25"/>
-      <c r="AP38" s="25"/>
-      <c r="AQ38" s="25"/>
-      <c r="AR38" s="25"/>
-      <c r="AS38" s="25"/>
-      <c r="AT38" s="25"/>
+      <c r="AO38" s="23"/>
+      <c r="AP38" s="23"/>
+      <c r="AQ38" s="23"/>
+      <c r="AR38" s="23"/>
+      <c r="AS38" s="23"/>
+      <c r="AT38" s="23"/>
     </row>
     <row r="39" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="39"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="22"/>
       <c r="P39" s="15"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="25"/>
-      <c r="U39" s="25"/>
-      <c r="V39" s="25"/>
-      <c r="W39" s="25"/>
-      <c r="X39" s="25"/>
-      <c r="Y39" s="25"/>
-      <c r="Z39" s="25"/>
-      <c r="AA39" s="25"/>
-      <c r="AB39" s="25"/>
-      <c r="AC39" s="25"/>
-      <c r="AD39" s="25"/>
-      <c r="AE39" s="25"/>
-      <c r="AF39" s="25"/>
-      <c r="AG39" s="25"/>
-      <c r="AH39" s="25"/>
-      <c r="AI39" s="25"/>
-      <c r="AJ39" s="25"/>
-      <c r="AK39" s="25"/>
-      <c r="AL39" s="25"/>
-      <c r="AM39" s="25"/>
-      <c r="AN39" s="25"/>
-      <c r="AO39" s="25"/>
-      <c r="AP39" s="25"/>
-      <c r="AQ39" s="25"/>
-      <c r="AR39" s="25"/>
-      <c r="AS39" s="25"/>
-      <c r="AT39" s="25"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="23"/>
+      <c r="W39" s="23"/>
+      <c r="X39" s="23"/>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="23"/>
+      <c r="AA39" s="23"/>
+      <c r="AB39" s="23"/>
+      <c r="AC39" s="23"/>
+      <c r="AD39" s="23"/>
+      <c r="AE39" s="23"/>
+      <c r="AF39" s="23"/>
+      <c r="AG39" s="23"/>
+      <c r="AH39" s="23"/>
+      <c r="AI39" s="23"/>
+      <c r="AJ39" s="23"/>
+      <c r="AK39" s="23"/>
+      <c r="AL39" s="23"/>
+      <c r="AM39" s="23"/>
+      <c r="AN39" s="23"/>
+      <c r="AO39" s="23"/>
+      <c r="AP39" s="23"/>
+      <c r="AQ39" s="23"/>
+      <c r="AR39" s="23"/>
+      <c r="AS39" s="23"/>
+      <c r="AT39" s="23"/>
     </row>
     <row r="40" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="39"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="22"/>
       <c r="P40" s="15"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-      <c r="T40" s="25"/>
-      <c r="U40" s="25"/>
-      <c r="V40" s="25"/>
-      <c r="W40" s="25"/>
-      <c r="X40" s="25"/>
-      <c r="Y40" s="25"/>
-      <c r="Z40" s="25"/>
-      <c r="AA40" s="25"/>
-      <c r="AB40" s="25"/>
-      <c r="AC40" s="25"/>
-      <c r="AD40" s="25"/>
-      <c r="AE40" s="25"/>
-      <c r="AF40" s="25"/>
-      <c r="AG40" s="25"/>
-      <c r="AH40" s="25"/>
-      <c r="AI40" s="25"/>
-      <c r="AJ40" s="25"/>
-      <c r="AK40" s="25"/>
-      <c r="AL40" s="25"/>
-      <c r="AM40" s="25"/>
-      <c r="AN40" s="25"/>
-      <c r="AO40" s="25"/>
-      <c r="AP40" s="25"/>
-      <c r="AQ40" s="25"/>
-      <c r="AR40" s="25"/>
-      <c r="AS40" s="25"/>
-      <c r="AT40" s="25"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="23"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
+      <c r="AA40" s="23"/>
+      <c r="AB40" s="23"/>
+      <c r="AC40" s="23"/>
+      <c r="AD40" s="23"/>
+      <c r="AE40" s="23"/>
+      <c r="AF40" s="23"/>
+      <c r="AG40" s="23"/>
+      <c r="AH40" s="23"/>
+      <c r="AI40" s="23"/>
+      <c r="AJ40" s="23"/>
+      <c r="AK40" s="23"/>
+      <c r="AL40" s="23"/>
+      <c r="AM40" s="23"/>
+      <c r="AN40" s="23"/>
+      <c r="AO40" s="23"/>
+      <c r="AP40" s="23"/>
+      <c r="AQ40" s="23"/>
+      <c r="AR40" s="23"/>
+      <c r="AS40" s="23"/>
+      <c r="AT40" s="23"/>
     </row>
     <row r="41" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="39"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="22"/>
       <c r="P41" s="15"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="25"/>
-      <c r="AA41" s="25"/>
-      <c r="AB41" s="25"/>
-      <c r="AC41" s="25"/>
-      <c r="AD41" s="25"/>
-      <c r="AE41" s="25"/>
-      <c r="AF41" s="25"/>
-      <c r="AG41" s="25"/>
-      <c r="AH41" s="25"/>
-      <c r="AI41" s="25"/>
-      <c r="AJ41" s="25"/>
-      <c r="AK41" s="25"/>
-      <c r="AL41" s="25"/>
-      <c r="AM41" s="25"/>
-      <c r="AN41" s="25"/>
-      <c r="AO41" s="25"/>
-      <c r="AP41" s="25"/>
-      <c r="AQ41" s="25"/>
-      <c r="AR41" s="25"/>
-      <c r="AS41" s="25"/>
-      <c r="AT41" s="25"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="23"/>
+      <c r="U41" s="23"/>
+      <c r="V41" s="23"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
+      <c r="Z41" s="23"/>
+      <c r="AA41" s="23"/>
+      <c r="AB41" s="23"/>
+      <c r="AC41" s="23"/>
+      <c r="AD41" s="23"/>
+      <c r="AE41" s="23"/>
+      <c r="AF41" s="23"/>
+      <c r="AG41" s="23"/>
+      <c r="AH41" s="23"/>
+      <c r="AI41" s="23"/>
+      <c r="AJ41" s="23"/>
+      <c r="AK41" s="23"/>
+      <c r="AL41" s="23"/>
+      <c r="AM41" s="23"/>
+      <c r="AN41" s="23"/>
+      <c r="AO41" s="23"/>
+      <c r="AP41" s="23"/>
+      <c r="AQ41" s="23"/>
+      <c r="AR41" s="23"/>
+      <c r="AS41" s="23"/>
+      <c r="AT41" s="23"/>
     </row>
     <row r="42" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="39"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="22"/>
       <c r="P42" s="15"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="25"/>
-      <c r="S42" s="25"/>
-      <c r="T42" s="25"/>
-      <c r="U42" s="25"/>
-      <c r="V42" s="25"/>
-      <c r="W42" s="25"/>
-      <c r="X42" s="25"/>
-      <c r="Y42" s="25"/>
-      <c r="Z42" s="25"/>
-      <c r="AA42" s="25"/>
-      <c r="AB42" s="25"/>
-      <c r="AC42" s="25"/>
-      <c r="AD42" s="25"/>
-      <c r="AE42" s="25"/>
-      <c r="AF42" s="25"/>
-      <c r="AG42" s="25"/>
-      <c r="AH42" s="25"/>
-      <c r="AI42" s="25"/>
-      <c r="AJ42" s="25"/>
-      <c r="AK42" s="25"/>
-      <c r="AL42" s="25"/>
-      <c r="AM42" s="25"/>
-      <c r="AN42" s="25"/>
-      <c r="AO42" s="25"/>
-      <c r="AP42" s="25"/>
-      <c r="AQ42" s="25"/>
-      <c r="AR42" s="25"/>
-      <c r="AS42" s="25"/>
-      <c r="AT42" s="25"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="23"/>
+      <c r="T42" s="23"/>
+      <c r="U42" s="23"/>
+      <c r="V42" s="23"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
+      <c r="Z42" s="23"/>
+      <c r="AA42" s="23"/>
+      <c r="AB42" s="23"/>
+      <c r="AC42" s="23"/>
+      <c r="AD42" s="23"/>
+      <c r="AE42" s="23"/>
+      <c r="AF42" s="23"/>
+      <c r="AG42" s="23"/>
+      <c r="AH42" s="23"/>
+      <c r="AI42" s="23"/>
+      <c r="AJ42" s="23"/>
+      <c r="AK42" s="23"/>
+      <c r="AL42" s="23"/>
+      <c r="AM42" s="23"/>
+      <c r="AN42" s="23"/>
+      <c r="AO42" s="23"/>
+      <c r="AP42" s="23"/>
+      <c r="AQ42" s="23"/>
+      <c r="AR42" s="23"/>
+      <c r="AS42" s="23"/>
+      <c r="AT42" s="23"/>
     </row>
     <row r="43" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="39"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="22"/>
       <c r="P43" s="15"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="25"/>
-      <c r="T43" s="25"/>
-      <c r="U43" s="25"/>
-      <c r="V43" s="25"/>
-      <c r="W43" s="25"/>
-      <c r="X43" s="25"/>
-      <c r="Y43" s="25"/>
-      <c r="Z43" s="25"/>
-      <c r="AA43" s="25"/>
-      <c r="AB43" s="25"/>
-      <c r="AC43" s="25"/>
-      <c r="AD43" s="25"/>
-      <c r="AE43" s="25"/>
-      <c r="AF43" s="25"/>
-      <c r="AG43" s="25"/>
-      <c r="AH43" s="25"/>
-      <c r="AI43" s="25"/>
-      <c r="AJ43" s="25"/>
-      <c r="AK43" s="25"/>
-      <c r="AL43" s="25"/>
-      <c r="AM43" s="25"/>
-      <c r="AN43" s="25"/>
-      <c r="AO43" s="25"/>
-      <c r="AP43" s="25"/>
-      <c r="AQ43" s="25"/>
-      <c r="AR43" s="25"/>
-      <c r="AS43" s="25"/>
-      <c r="AT43" s="25"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="23"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
+      <c r="Z43" s="23"/>
+      <c r="AA43" s="23"/>
+      <c r="AB43" s="23"/>
+      <c r="AC43" s="23"/>
+      <c r="AD43" s="23"/>
+      <c r="AE43" s="23"/>
+      <c r="AF43" s="23"/>
+      <c r="AG43" s="23"/>
+      <c r="AH43" s="23"/>
+      <c r="AI43" s="23"/>
+      <c r="AJ43" s="23"/>
+      <c r="AK43" s="23"/>
+      <c r="AL43" s="23"/>
+      <c r="AM43" s="23"/>
+      <c r="AN43" s="23"/>
+      <c r="AO43" s="23"/>
+      <c r="AP43" s="23"/>
+      <c r="AQ43" s="23"/>
+      <c r="AR43" s="23"/>
+      <c r="AS43" s="23"/>
+      <c r="AT43" s="23"/>
     </row>
     <row r="44" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-      <c r="O44" s="39"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="22"/>
       <c r="P44" s="15"/>
-      <c r="Q44" s="25"/>
-      <c r="R44" s="25"/>
-      <c r="S44" s="25"/>
-      <c r="T44" s="25"/>
-      <c r="U44" s="25"/>
-      <c r="V44" s="25"/>
-      <c r="W44" s="25"/>
-      <c r="X44" s="25"/>
-      <c r="Y44" s="25"/>
-      <c r="Z44" s="25"/>
-      <c r="AA44" s="25"/>
-      <c r="AB44" s="25"/>
-      <c r="AC44" s="25"/>
-      <c r="AD44" s="25"/>
-      <c r="AE44" s="25"/>
-      <c r="AF44" s="25"/>
-      <c r="AG44" s="25"/>
-      <c r="AH44" s="25"/>
-      <c r="AI44" s="25"/>
-      <c r="AJ44" s="25"/>
-      <c r="AK44" s="25"/>
-      <c r="AL44" s="25"/>
-      <c r="AM44" s="25"/>
-      <c r="AN44" s="25"/>
-      <c r="AO44" s="25"/>
-      <c r="AP44" s="25"/>
-      <c r="AQ44" s="25"/>
-      <c r="AR44" s="25"/>
-      <c r="AS44" s="25"/>
-      <c r="AT44" s="25"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="23"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
+      <c r="Z44" s="23"/>
+      <c r="AA44" s="23"/>
+      <c r="AB44" s="23"/>
+      <c r="AC44" s="23"/>
+      <c r="AD44" s="23"/>
+      <c r="AE44" s="23"/>
+      <c r="AF44" s="23"/>
+      <c r="AG44" s="23"/>
+      <c r="AH44" s="23"/>
+      <c r="AI44" s="23"/>
+      <c r="AJ44" s="23"/>
+      <c r="AK44" s="23"/>
+      <c r="AL44" s="23"/>
+      <c r="AM44" s="23"/>
+      <c r="AN44" s="23"/>
+      <c r="AO44" s="23"/>
+      <c r="AP44" s="23"/>
+      <c r="AQ44" s="23"/>
+      <c r="AR44" s="23"/>
+      <c r="AS44" s="23"/>
+      <c r="AT44" s="23"/>
     </row>
     <row r="45" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="39"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="22"/>
       <c r="P45" s="15"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-      <c r="T45" s="25"/>
-      <c r="U45" s="25"/>
-      <c r="V45" s="25"/>
-      <c r="W45" s="25"/>
-      <c r="X45" s="25"/>
-      <c r="Y45" s="25"/>
-      <c r="Z45" s="25"/>
-      <c r="AA45" s="25"/>
-      <c r="AB45" s="25"/>
-      <c r="AC45" s="25"/>
-      <c r="AD45" s="25"/>
-      <c r="AE45" s="25"/>
-      <c r="AF45" s="25"/>
-      <c r="AG45" s="25"/>
-      <c r="AH45" s="25"/>
-      <c r="AI45" s="25"/>
-      <c r="AJ45" s="25"/>
-      <c r="AK45" s="25"/>
-      <c r="AL45" s="25"/>
-      <c r="AM45" s="25"/>
-      <c r="AN45" s="25"/>
-      <c r="AO45" s="25"/>
-      <c r="AP45" s="25"/>
-      <c r="AQ45" s="25"/>
-      <c r="AR45" s="25"/>
-      <c r="AS45" s="25"/>
-      <c r="AT45" s="25"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="23"/>
+      <c r="S45" s="23"/>
+      <c r="T45" s="23"/>
+      <c r="U45" s="23"/>
+      <c r="V45" s="23"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
+      <c r="Z45" s="23"/>
+      <c r="AA45" s="23"/>
+      <c r="AB45" s="23"/>
+      <c r="AC45" s="23"/>
+      <c r="AD45" s="23"/>
+      <c r="AE45" s="23"/>
+      <c r="AF45" s="23"/>
+      <c r="AG45" s="23"/>
+      <c r="AH45" s="23"/>
+      <c r="AI45" s="23"/>
+      <c r="AJ45" s="23"/>
+      <c r="AK45" s="23"/>
+      <c r="AL45" s="23"/>
+      <c r="AM45" s="23"/>
+      <c r="AN45" s="23"/>
+      <c r="AO45" s="23"/>
+      <c r="AP45" s="23"/>
+      <c r="AQ45" s="23"/>
+      <c r="AR45" s="23"/>
+      <c r="AS45" s="23"/>
+      <c r="AT45" s="23"/>
     </row>
     <row r="46" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="39"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="22"/>
       <c r="P46" s="15"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25"/>
-      <c r="T46" s="25"/>
-      <c r="U46" s="25"/>
-      <c r="V46" s="25"/>
-      <c r="W46" s="25"/>
-      <c r="X46" s="25"/>
-      <c r="Y46" s="25"/>
-      <c r="Z46" s="25"/>
-      <c r="AA46" s="25"/>
-      <c r="AB46" s="25"/>
-      <c r="AC46" s="25"/>
-      <c r="AD46" s="25"/>
-      <c r="AE46" s="25"/>
-      <c r="AF46" s="25"/>
-      <c r="AG46" s="25"/>
-      <c r="AH46" s="25"/>
-      <c r="AI46" s="25"/>
-      <c r="AJ46" s="25"/>
-      <c r="AK46" s="25"/>
-      <c r="AL46" s="25"/>
-      <c r="AM46" s="25"/>
-      <c r="AN46" s="25"/>
-      <c r="AO46" s="25"/>
-      <c r="AP46" s="25"/>
-      <c r="AQ46" s="25"/>
-      <c r="AR46" s="25"/>
-      <c r="AS46" s="25"/>
-      <c r="AT46" s="25"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="23"/>
+      <c r="S46" s="23"/>
+      <c r="T46" s="23"/>
+      <c r="U46" s="23"/>
+      <c r="V46" s="23"/>
+      <c r="W46" s="23"/>
+      <c r="X46" s="23"/>
+      <c r="Y46" s="23"/>
+      <c r="Z46" s="23"/>
+      <c r="AA46" s="23"/>
+      <c r="AB46" s="23"/>
+      <c r="AC46" s="23"/>
+      <c r="AD46" s="23"/>
+      <c r="AE46" s="23"/>
+      <c r="AF46" s="23"/>
+      <c r="AG46" s="23"/>
+      <c r="AH46" s="23"/>
+      <c r="AI46" s="23"/>
+      <c r="AJ46" s="23"/>
+      <c r="AK46" s="23"/>
+      <c r="AL46" s="23"/>
+      <c r="AM46" s="23"/>
+      <c r="AN46" s="23"/>
+      <c r="AO46" s="23"/>
+      <c r="AP46" s="23"/>
+      <c r="AQ46" s="23"/>
+      <c r="AR46" s="23"/>
+      <c r="AS46" s="23"/>
+      <c r="AT46" s="23"/>
     </row>
     <row r="47" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="39"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="22"/>
       <c r="P47" s="15"/>
-      <c r="Q47" s="25"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="25"/>
-      <c r="T47" s="25"/>
-      <c r="U47" s="25"/>
-      <c r="V47" s="25"/>
-      <c r="W47" s="25"/>
-      <c r="X47" s="25"/>
-      <c r="Y47" s="25"/>
-      <c r="Z47" s="25"/>
-      <c r="AA47" s="25"/>
-      <c r="AB47" s="25"/>
-      <c r="AC47" s="25"/>
-      <c r="AD47" s="25"/>
-      <c r="AE47" s="25"/>
-      <c r="AF47" s="25"/>
-      <c r="AG47" s="25"/>
-      <c r="AH47" s="25"/>
-      <c r="AI47" s="25"/>
-      <c r="AJ47" s="25"/>
-      <c r="AK47" s="25"/>
-      <c r="AL47" s="25"/>
-      <c r="AM47" s="25"/>
-      <c r="AN47" s="25"/>
-      <c r="AO47" s="25"/>
-      <c r="AP47" s="25"/>
-      <c r="AQ47" s="25"/>
-      <c r="AR47" s="25"/>
-      <c r="AS47" s="25"/>
-      <c r="AT47" s="25"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="23"/>
+      <c r="S47" s="23"/>
+      <c r="T47" s="23"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="23"/>
+      <c r="W47" s="23"/>
+      <c r="X47" s="23"/>
+      <c r="Y47" s="23"/>
+      <c r="Z47" s="23"/>
+      <c r="AA47" s="23"/>
+      <c r="AB47" s="23"/>
+      <c r="AC47" s="23"/>
+      <c r="AD47" s="23"/>
+      <c r="AE47" s="23"/>
+      <c r="AF47" s="23"/>
+      <c r="AG47" s="23"/>
+      <c r="AH47" s="23"/>
+      <c r="AI47" s="23"/>
+      <c r="AJ47" s="23"/>
+      <c r="AK47" s="23"/>
+      <c r="AL47" s="23"/>
+      <c r="AM47" s="23"/>
+      <c r="AN47" s="23"/>
+      <c r="AO47" s="23"/>
+      <c r="AP47" s="23"/>
+      <c r="AQ47" s="23"/>
+      <c r="AR47" s="23"/>
+      <c r="AS47" s="23"/>
+      <c r="AT47" s="23"/>
     </row>
     <row r="48" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="39"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="22"/>
       <c r="P48" s="15"/>
-      <c r="Q48" s="25"/>
-      <c r="R48" s="25"/>
-      <c r="S48" s="25"/>
-      <c r="T48" s="25"/>
-      <c r="U48" s="25"/>
-      <c r="V48" s="25"/>
-      <c r="W48" s="25"/>
-      <c r="X48" s="25"/>
-      <c r="Y48" s="25"/>
-      <c r="Z48" s="25"/>
-      <c r="AA48" s="25"/>
-      <c r="AB48" s="25"/>
-      <c r="AC48" s="25"/>
-      <c r="AD48" s="25"/>
-      <c r="AE48" s="25"/>
-      <c r="AF48" s="25"/>
-      <c r="AG48" s="25"/>
-      <c r="AH48" s="25"/>
-      <c r="AI48" s="25"/>
-      <c r="AJ48" s="25"/>
-      <c r="AK48" s="25"/>
-      <c r="AL48" s="25"/>
-      <c r="AM48" s="25"/>
-      <c r="AN48" s="25"/>
-      <c r="AO48" s="25"/>
-      <c r="AP48" s="25"/>
-      <c r="AQ48" s="25"/>
-      <c r="AR48" s="25"/>
-      <c r="AS48" s="25"/>
-      <c r="AT48" s="25"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="23"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="23"/>
+      <c r="U48" s="23"/>
+      <c r="V48" s="23"/>
+      <c r="W48" s="23"/>
+      <c r="X48" s="23"/>
+      <c r="Y48" s="23"/>
+      <c r="Z48" s="23"/>
+      <c r="AA48" s="23"/>
+      <c r="AB48" s="23"/>
+      <c r="AC48" s="23"/>
+      <c r="AD48" s="23"/>
+      <c r="AE48" s="23"/>
+      <c r="AF48" s="23"/>
+      <c r="AG48" s="23"/>
+      <c r="AH48" s="23"/>
+      <c r="AI48" s="23"/>
+      <c r="AJ48" s="23"/>
+      <c r="AK48" s="23"/>
+      <c r="AL48" s="23"/>
+      <c r="AM48" s="23"/>
+      <c r="AN48" s="23"/>
+      <c r="AO48" s="23"/>
+      <c r="AP48" s="23"/>
+      <c r="AQ48" s="23"/>
+      <c r="AR48" s="23"/>
+      <c r="AS48" s="23"/>
+      <c r="AT48" s="23"/>
     </row>
     <row r="49" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
-      <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
-      <c r="O49" s="39"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="22"/>
       <c r="P49" s="15"/>
-      <c r="Q49" s="25"/>
-      <c r="R49" s="25"/>
-      <c r="S49" s="25"/>
-      <c r="T49" s="25"/>
-      <c r="U49" s="25"/>
-      <c r="V49" s="25"/>
-      <c r="W49" s="25"/>
-      <c r="X49" s="25"/>
-      <c r="Y49" s="25"/>
-      <c r="Z49" s="25"/>
-      <c r="AA49" s="25"/>
-      <c r="AB49" s="25"/>
-      <c r="AC49" s="25"/>
-      <c r="AD49" s="25"/>
-      <c r="AE49" s="25"/>
-      <c r="AF49" s="25"/>
-      <c r="AG49" s="25"/>
-      <c r="AH49" s="25"/>
-      <c r="AI49" s="25"/>
-      <c r="AJ49" s="25"/>
-      <c r="AK49" s="25"/>
-      <c r="AL49" s="25"/>
-      <c r="AM49" s="25"/>
-      <c r="AN49" s="25"/>
-      <c r="AO49" s="25"/>
-      <c r="AP49" s="25"/>
-      <c r="AQ49" s="25"/>
-      <c r="AR49" s="25"/>
-      <c r="AS49" s="25"/>
-      <c r="AT49" s="25"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="23"/>
+      <c r="S49" s="23"/>
+      <c r="T49" s="23"/>
+      <c r="U49" s="23"/>
+      <c r="V49" s="23"/>
+      <c r="W49" s="23"/>
+      <c r="X49" s="23"/>
+      <c r="Y49" s="23"/>
+      <c r="Z49" s="23"/>
+      <c r="AA49" s="23"/>
+      <c r="AB49" s="23"/>
+      <c r="AC49" s="23"/>
+      <c r="AD49" s="23"/>
+      <c r="AE49" s="23"/>
+      <c r="AF49" s="23"/>
+      <c r="AG49" s="23"/>
+      <c r="AH49" s="23"/>
+      <c r="AI49" s="23"/>
+      <c r="AJ49" s="23"/>
+      <c r="AK49" s="23"/>
+      <c r="AL49" s="23"/>
+      <c r="AM49" s="23"/>
+      <c r="AN49" s="23"/>
+      <c r="AO49" s="23"/>
+      <c r="AP49" s="23"/>
+      <c r="AQ49" s="23"/>
+      <c r="AR49" s="23"/>
+      <c r="AS49" s="23"/>
+      <c r="AT49" s="23"/>
     </row>
     <row r="50" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
-      <c r="M50" s="27"/>
-      <c r="N50" s="27"/>
-      <c r="O50" s="39"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="22"/>
       <c r="P50" s="15"/>
-      <c r="Q50" s="25"/>
-      <c r="R50" s="25"/>
-      <c r="S50" s="25"/>
-      <c r="T50" s="25"/>
-      <c r="U50" s="25"/>
-      <c r="V50" s="25"/>
-      <c r="W50" s="25"/>
-      <c r="X50" s="25"/>
-      <c r="Y50" s="25"/>
-      <c r="Z50" s="25"/>
-      <c r="AA50" s="25"/>
-      <c r="AB50" s="25"/>
-      <c r="AC50" s="25"/>
-      <c r="AD50" s="25"/>
-      <c r="AE50" s="25"/>
-      <c r="AF50" s="25"/>
-      <c r="AG50" s="25"/>
-      <c r="AH50" s="25"/>
-      <c r="AI50" s="25"/>
-      <c r="AJ50" s="25"/>
-      <c r="AK50" s="25"/>
-      <c r="AL50" s="25"/>
-      <c r="AM50" s="25"/>
-      <c r="AN50" s="25"/>
-      <c r="AO50" s="25"/>
-      <c r="AP50" s="25"/>
-      <c r="AQ50" s="25"/>
-      <c r="AR50" s="25"/>
-      <c r="AS50" s="25"/>
-      <c r="AT50" s="25"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="23"/>
+      <c r="T50" s="23"/>
+      <c r="U50" s="23"/>
+      <c r="V50" s="23"/>
+      <c r="W50" s="23"/>
+      <c r="X50" s="23"/>
+      <c r="Y50" s="23"/>
+      <c r="Z50" s="23"/>
+      <c r="AA50" s="23"/>
+      <c r="AB50" s="23"/>
+      <c r="AC50" s="23"/>
+      <c r="AD50" s="23"/>
+      <c r="AE50" s="23"/>
+      <c r="AF50" s="23"/>
+      <c r="AG50" s="23"/>
+      <c r="AH50" s="23"/>
+      <c r="AI50" s="23"/>
+      <c r="AJ50" s="23"/>
+      <c r="AK50" s="23"/>
+      <c r="AL50" s="23"/>
+      <c r="AM50" s="23"/>
+      <c r="AN50" s="23"/>
+      <c r="AO50" s="23"/>
+      <c r="AP50" s="23"/>
+      <c r="AQ50" s="23"/>
+      <c r="AR50" s="23"/>
+      <c r="AS50" s="23"/>
+      <c r="AT50" s="23"/>
     </row>
     <row r="51" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="27"/>
-      <c r="N51" s="27"/>
-      <c r="O51" s="39"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="22"/>
       <c r="P51" s="15"/>
-      <c r="Q51" s="25"/>
-      <c r="R51" s="25"/>
-      <c r="S51" s="25"/>
-      <c r="T51" s="25"/>
-      <c r="U51" s="25"/>
-      <c r="V51" s="25"/>
-      <c r="W51" s="25"/>
-      <c r="X51" s="25"/>
-      <c r="Y51" s="25"/>
-      <c r="Z51" s="25"/>
-      <c r="AA51" s="25"/>
-      <c r="AB51" s="25"/>
-      <c r="AC51" s="25"/>
-      <c r="AD51" s="25"/>
-      <c r="AE51" s="25"/>
-      <c r="AF51" s="25"/>
-      <c r="AG51" s="25"/>
-      <c r="AH51" s="25"/>
-      <c r="AI51" s="25"/>
-      <c r="AJ51" s="25"/>
-      <c r="AK51" s="25"/>
-      <c r="AL51" s="25"/>
-      <c r="AM51" s="25"/>
-      <c r="AN51" s="25"/>
-      <c r="AO51" s="25"/>
-      <c r="AP51" s="25"/>
-      <c r="AQ51" s="25"/>
-      <c r="AR51" s="25"/>
-      <c r="AS51" s="25"/>
-      <c r="AT51" s="25"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="23"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="23"/>
+      <c r="W51" s="23"/>
+      <c r="X51" s="23"/>
+      <c r="Y51" s="23"/>
+      <c r="Z51" s="23"/>
+      <c r="AA51" s="23"/>
+      <c r="AB51" s="23"/>
+      <c r="AC51" s="23"/>
+      <c r="AD51" s="23"/>
+      <c r="AE51" s="23"/>
+      <c r="AF51" s="23"/>
+      <c r="AG51" s="23"/>
+      <c r="AH51" s="23"/>
+      <c r="AI51" s="23"/>
+      <c r="AJ51" s="23"/>
+      <c r="AK51" s="23"/>
+      <c r="AL51" s="23"/>
+      <c r="AM51" s="23"/>
+      <c r="AN51" s="23"/>
+      <c r="AO51" s="23"/>
+      <c r="AP51" s="23"/>
+      <c r="AQ51" s="23"/>
+      <c r="AR51" s="23"/>
+      <c r="AS51" s="23"/>
+      <c r="AT51" s="23"/>
     </row>
     <row r="52" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
-      <c r="M52" s="27"/>
-      <c r="N52" s="27"/>
-      <c r="O52" s="39"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="22"/>
       <c r="P52" s="15"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="25"/>
-      <c r="T52" s="25"/>
-      <c r="U52" s="25"/>
-      <c r="V52" s="25"/>
-      <c r="W52" s="25"/>
-      <c r="X52" s="25"/>
-      <c r="Y52" s="25"/>
-      <c r="Z52" s="25"/>
-      <c r="AA52" s="25"/>
-      <c r="AB52" s="25"/>
-      <c r="AC52" s="25"/>
-      <c r="AD52" s="25"/>
-      <c r="AE52" s="25"/>
-      <c r="AF52" s="25"/>
-      <c r="AG52" s="25"/>
-      <c r="AH52" s="25"/>
-      <c r="AI52" s="25"/>
-      <c r="AJ52" s="25"/>
-      <c r="AK52" s="25"/>
-      <c r="AL52" s="25"/>
-      <c r="AM52" s="25"/>
-      <c r="AN52" s="25"/>
-      <c r="AO52" s="25"/>
-      <c r="AP52" s="25"/>
-      <c r="AQ52" s="25"/>
-      <c r="AR52" s="25"/>
-      <c r="AS52" s="25"/>
-      <c r="AT52" s="25"/>
+      <c r="Q52" s="23"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="23"/>
+      <c r="T52" s="23"/>
+      <c r="U52" s="23"/>
+      <c r="V52" s="23"/>
+      <c r="W52" s="23"/>
+      <c r="X52" s="23"/>
+      <c r="Y52" s="23"/>
+      <c r="Z52" s="23"/>
+      <c r="AA52" s="23"/>
+      <c r="AB52" s="23"/>
+      <c r="AC52" s="23"/>
+      <c r="AD52" s="23"/>
+      <c r="AE52" s="23"/>
+      <c r="AF52" s="23"/>
+      <c r="AG52" s="23"/>
+      <c r="AH52" s="23"/>
+      <c r="AI52" s="23"/>
+      <c r="AJ52" s="23"/>
+      <c r="AK52" s="23"/>
+      <c r="AL52" s="23"/>
+      <c r="AM52" s="23"/>
+      <c r="AN52" s="23"/>
+      <c r="AO52" s="23"/>
+      <c r="AP52" s="23"/>
+      <c r="AQ52" s="23"/>
+      <c r="AR52" s="23"/>
+      <c r="AS52" s="23"/>
+      <c r="AT52" s="23"/>
     </row>
     <row r="53" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-      <c r="L53" s="27"/>
-      <c r="M53" s="27"/>
-      <c r="N53" s="27"/>
-      <c r="O53" s="39"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="22"/>
       <c r="P53" s="15"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="25"/>
-      <c r="T53" s="25"/>
-      <c r="U53" s="25"/>
-      <c r="V53" s="25"/>
-      <c r="W53" s="25"/>
-      <c r="X53" s="25"/>
-      <c r="Y53" s="25"/>
-      <c r="Z53" s="25"/>
-      <c r="AA53" s="25"/>
-      <c r="AB53" s="25"/>
-      <c r="AC53" s="25"/>
-      <c r="AD53" s="25"/>
-      <c r="AE53" s="25"/>
-      <c r="AF53" s="25"/>
-      <c r="AG53" s="25"/>
-      <c r="AH53" s="25"/>
-      <c r="AI53" s="25"/>
-      <c r="AJ53" s="25"/>
-      <c r="AK53" s="25"/>
-      <c r="AL53" s="25"/>
-      <c r="AM53" s="25"/>
-      <c r="AN53" s="25"/>
-      <c r="AO53" s="25"/>
-      <c r="AP53" s="25"/>
-      <c r="AQ53" s="25"/>
-      <c r="AR53" s="25"/>
-      <c r="AS53" s="25"/>
-      <c r="AT53" s="25"/>
+      <c r="Q53" s="23"/>
+      <c r="R53" s="23"/>
+      <c r="S53" s="23"/>
+      <c r="T53" s="23"/>
+      <c r="U53" s="23"/>
+      <c r="V53" s="23"/>
+      <c r="W53" s="23"/>
+      <c r="X53" s="23"/>
+      <c r="Y53" s="23"/>
+      <c r="Z53" s="23"/>
+      <c r="AA53" s="23"/>
+      <c r="AB53" s="23"/>
+      <c r="AC53" s="23"/>
+      <c r="AD53" s="23"/>
+      <c r="AE53" s="23"/>
+      <c r="AF53" s="23"/>
+      <c r="AG53" s="23"/>
+      <c r="AH53" s="23"/>
+      <c r="AI53" s="23"/>
+      <c r="AJ53" s="23"/>
+      <c r="AK53" s="23"/>
+      <c r="AL53" s="23"/>
+      <c r="AM53" s="23"/>
+      <c r="AN53" s="23"/>
+      <c r="AO53" s="23"/>
+      <c r="AP53" s="23"/>
+      <c r="AQ53" s="23"/>
+      <c r="AR53" s="23"/>
+      <c r="AS53" s="23"/>
+      <c r="AT53" s="23"/>
     </row>
     <row r="54" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="27"/>
-      <c r="O54" s="39"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="22"/>
       <c r="P54" s="15"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="25"/>
-      <c r="T54" s="25"/>
-      <c r="U54" s="25"/>
-      <c r="V54" s="25"/>
-      <c r="W54" s="25"/>
-      <c r="X54" s="25"/>
-      <c r="Y54" s="25"/>
-      <c r="Z54" s="25"/>
-      <c r="AA54" s="25"/>
-      <c r="AB54" s="25"/>
-      <c r="AC54" s="25"/>
-      <c r="AD54" s="25"/>
-      <c r="AE54" s="25"/>
-      <c r="AF54" s="25"/>
-      <c r="AG54" s="25"/>
-      <c r="AH54" s="25"/>
-      <c r="AI54" s="25"/>
-      <c r="AJ54" s="25"/>
-      <c r="AK54" s="25"/>
-      <c r="AL54" s="25"/>
-      <c r="AM54" s="25"/>
-      <c r="AN54" s="25"/>
-      <c r="AO54" s="25"/>
-      <c r="AP54" s="25"/>
-      <c r="AQ54" s="25"/>
-      <c r="AR54" s="25"/>
-      <c r="AS54" s="25"/>
-      <c r="AT54" s="25"/>
+      <c r="Q54" s="23"/>
+      <c r="R54" s="23"/>
+      <c r="S54" s="23"/>
+      <c r="T54" s="23"/>
+      <c r="U54" s="23"/>
+      <c r="V54" s="23"/>
+      <c r="W54" s="23"/>
+      <c r="X54" s="23"/>
+      <c r="Y54" s="23"/>
+      <c r="Z54" s="23"/>
+      <c r="AA54" s="23"/>
+      <c r="AB54" s="23"/>
+      <c r="AC54" s="23"/>
+      <c r="AD54" s="23"/>
+      <c r="AE54" s="23"/>
+      <c r="AF54" s="23"/>
+      <c r="AG54" s="23"/>
+      <c r="AH54" s="23"/>
+      <c r="AI54" s="23"/>
+      <c r="AJ54" s="23"/>
+      <c r="AK54" s="23"/>
+      <c r="AL54" s="23"/>
+      <c r="AM54" s="23"/>
+      <c r="AN54" s="23"/>
+      <c r="AO54" s="23"/>
+      <c r="AP54" s="23"/>
+      <c r="AQ54" s="23"/>
+      <c r="AR54" s="23"/>
+      <c r="AS54" s="23"/>
+      <c r="AT54" s="23"/>
     </row>
     <row r="55" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="27"/>
-      <c r="K55" s="27"/>
-      <c r="L55" s="27"/>
-      <c r="M55" s="27"/>
-      <c r="N55" s="27"/>
-      <c r="O55" s="39"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="22"/>
       <c r="P55" s="15"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="25"/>
-      <c r="T55" s="25"/>
-      <c r="U55" s="25"/>
-      <c r="V55" s="25"/>
-      <c r="W55" s="25"/>
-      <c r="X55" s="25"/>
-      <c r="Y55" s="25"/>
-      <c r="Z55" s="25"/>
-      <c r="AA55" s="25"/>
-      <c r="AB55" s="25"/>
-      <c r="AC55" s="25"/>
-      <c r="AD55" s="25"/>
-      <c r="AE55" s="25"/>
-      <c r="AF55" s="25"/>
-      <c r="AG55" s="25"/>
-      <c r="AH55" s="25"/>
-      <c r="AI55" s="25"/>
-      <c r="AJ55" s="25"/>
-      <c r="AK55" s="25"/>
-      <c r="AL55" s="25"/>
-      <c r="AM55" s="25"/>
-      <c r="AN55" s="25"/>
-      <c r="AO55" s="25"/>
-      <c r="AP55" s="25"/>
-      <c r="AQ55" s="25"/>
-      <c r="AR55" s="25"/>
-      <c r="AS55" s="25"/>
-      <c r="AT55" s="25"/>
+      <c r="Q55" s="23"/>
+      <c r="R55" s="23"/>
+      <c r="S55" s="23"/>
+      <c r="T55" s="23"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="23"/>
+      <c r="W55" s="23"/>
+      <c r="X55" s="23"/>
+      <c r="Y55" s="23"/>
+      <c r="Z55" s="23"/>
+      <c r="AA55" s="23"/>
+      <c r="AB55" s="23"/>
+      <c r="AC55" s="23"/>
+      <c r="AD55" s="23"/>
+      <c r="AE55" s="23"/>
+      <c r="AF55" s="23"/>
+      <c r="AG55" s="23"/>
+      <c r="AH55" s="23"/>
+      <c r="AI55" s="23"/>
+      <c r="AJ55" s="23"/>
+      <c r="AK55" s="23"/>
+      <c r="AL55" s="23"/>
+      <c r="AM55" s="23"/>
+      <c r="AN55" s="23"/>
+      <c r="AO55" s="23"/>
+      <c r="AP55" s="23"/>
+      <c r="AQ55" s="23"/>
+      <c r="AR55" s="23"/>
+      <c r="AS55" s="23"/>
+      <c r="AT55" s="23"/>
     </row>
     <row r="56" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="39"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="22"/>
       <c r="P56" s="15"/>
-      <c r="Q56" s="25"/>
-      <c r="R56" s="25"/>
-      <c r="S56" s="25"/>
-      <c r="T56" s="25"/>
-      <c r="U56" s="25"/>
-      <c r="V56" s="25"/>
-      <c r="W56" s="25"/>
-      <c r="X56" s="25"/>
-      <c r="Y56" s="25"/>
-      <c r="Z56" s="25"/>
-      <c r="AA56" s="25"/>
-      <c r="AB56" s="25"/>
-      <c r="AC56" s="25"/>
-      <c r="AD56" s="25"/>
-      <c r="AE56" s="25"/>
-      <c r="AF56" s="25"/>
-      <c r="AG56" s="25"/>
-      <c r="AH56" s="25"/>
-      <c r="AI56" s="25"/>
-      <c r="AJ56" s="25"/>
-      <c r="AK56" s="25"/>
-      <c r="AL56" s="25"/>
-      <c r="AM56" s="25"/>
-      <c r="AN56" s="25"/>
-      <c r="AO56" s="25"/>
-      <c r="AP56" s="25"/>
-      <c r="AQ56" s="25"/>
-      <c r="AR56" s="25"/>
-      <c r="AS56" s="25"/>
-      <c r="AT56" s="25"/>
+      <c r="Q56" s="23"/>
+      <c r="R56" s="23"/>
+      <c r="S56" s="23"/>
+      <c r="T56" s="23"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="23"/>
+      <c r="W56" s="23"/>
+      <c r="X56" s="23"/>
+      <c r="Y56" s="23"/>
+      <c r="Z56" s="23"/>
+      <c r="AA56" s="23"/>
+      <c r="AB56" s="23"/>
+      <c r="AC56" s="23"/>
+      <c r="AD56" s="23"/>
+      <c r="AE56" s="23"/>
+      <c r="AF56" s="23"/>
+      <c r="AG56" s="23"/>
+      <c r="AH56" s="23"/>
+      <c r="AI56" s="23"/>
+      <c r="AJ56" s="23"/>
+      <c r="AK56" s="23"/>
+      <c r="AL56" s="23"/>
+      <c r="AM56" s="23"/>
+      <c r="AN56" s="23"/>
+      <c r="AO56" s="23"/>
+      <c r="AP56" s="23"/>
+      <c r="AQ56" s="23"/>
+      <c r="AR56" s="23"/>
+      <c r="AS56" s="23"/>
+      <c r="AT56" s="23"/>
     </row>
     <row r="57" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="27"/>
-      <c r="L57" s="27"/>
-      <c r="M57" s="27"/>
-      <c r="N57" s="27"/>
-      <c r="O57" s="39"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="22"/>
       <c r="P57" s="15"/>
-      <c r="Q57" s="25"/>
-      <c r="R57" s="25"/>
-      <c r="S57" s="25"/>
-      <c r="T57" s="25"/>
-      <c r="U57" s="25"/>
-      <c r="V57" s="25"/>
-      <c r="W57" s="25"/>
-      <c r="X57" s="25"/>
-      <c r="Y57" s="25"/>
-      <c r="Z57" s="25"/>
-      <c r="AA57" s="25"/>
-      <c r="AB57" s="25"/>
-      <c r="AC57" s="25"/>
-      <c r="AD57" s="25"/>
-      <c r="AE57" s="25"/>
-      <c r="AF57" s="25"/>
-      <c r="AG57" s="25"/>
-      <c r="AH57" s="25"/>
-      <c r="AI57" s="25"/>
-      <c r="AJ57" s="25"/>
-      <c r="AK57" s="25"/>
-      <c r="AL57" s="25"/>
-      <c r="AM57" s="25"/>
-      <c r="AN57" s="25"/>
-      <c r="AO57" s="25"/>
-      <c r="AP57" s="25"/>
-      <c r="AQ57" s="25"/>
-      <c r="AR57" s="25"/>
-      <c r="AS57" s="25"/>
-      <c r="AT57" s="25"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="23"/>
+      <c r="S57" s="23"/>
+      <c r="T57" s="23"/>
+      <c r="U57" s="23"/>
+      <c r="V57" s="23"/>
+      <c r="W57" s="23"/>
+      <c r="X57" s="23"/>
+      <c r="Y57" s="23"/>
+      <c r="Z57" s="23"/>
+      <c r="AA57" s="23"/>
+      <c r="AB57" s="23"/>
+      <c r="AC57" s="23"/>
+      <c r="AD57" s="23"/>
+      <c r="AE57" s="23"/>
+      <c r="AF57" s="23"/>
+      <c r="AG57" s="23"/>
+      <c r="AH57" s="23"/>
+      <c r="AI57" s="23"/>
+      <c r="AJ57" s="23"/>
+      <c r="AK57" s="23"/>
+      <c r="AL57" s="23"/>
+      <c r="AM57" s="23"/>
+      <c r="AN57" s="23"/>
+      <c r="AO57" s="23"/>
+      <c r="AP57" s="23"/>
+      <c r="AQ57" s="23"/>
+      <c r="AR57" s="23"/>
+      <c r="AS57" s="23"/>
+      <c r="AT57" s="23"/>
     </row>
     <row r="58" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
-      <c r="K58" s="27"/>
-      <c r="L58" s="27"/>
-      <c r="M58" s="27"/>
-      <c r="N58" s="27"/>
-      <c r="O58" s="39"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="22"/>
       <c r="P58" s="15"/>
-      <c r="Q58" s="25"/>
-      <c r="R58" s="25"/>
-      <c r="S58" s="25"/>
-      <c r="T58" s="25"/>
-      <c r="U58" s="25"/>
-      <c r="V58" s="25"/>
-      <c r="W58" s="25"/>
-      <c r="X58" s="25"/>
-      <c r="Y58" s="25"/>
-      <c r="Z58" s="25"/>
-      <c r="AA58" s="25"/>
-      <c r="AB58" s="25"/>
-      <c r="AC58" s="25"/>
-      <c r="AD58" s="25"/>
-      <c r="AE58" s="25"/>
-      <c r="AF58" s="25"/>
-      <c r="AG58" s="25"/>
-      <c r="AH58" s="25"/>
-      <c r="AI58" s="25"/>
-      <c r="AJ58" s="25"/>
-      <c r="AK58" s="25"/>
-      <c r="AL58" s="25"/>
-      <c r="AM58" s="25"/>
-      <c r="AN58" s="25"/>
-      <c r="AO58" s="25"/>
-      <c r="AP58" s="25"/>
-      <c r="AQ58" s="25"/>
-      <c r="AR58" s="25"/>
-      <c r="AS58" s="25"/>
-      <c r="AT58" s="25"/>
+      <c r="Q58" s="23"/>
+      <c r="R58" s="23"/>
+      <c r="S58" s="23"/>
+      <c r="T58" s="23"/>
+      <c r="U58" s="23"/>
+      <c r="V58" s="23"/>
+      <c r="W58" s="23"/>
+      <c r="X58" s="23"/>
+      <c r="Y58" s="23"/>
+      <c r="Z58" s="23"/>
+      <c r="AA58" s="23"/>
+      <c r="AB58" s="23"/>
+      <c r="AC58" s="23"/>
+      <c r="AD58" s="23"/>
+      <c r="AE58" s="23"/>
+      <c r="AF58" s="23"/>
+      <c r="AG58" s="23"/>
+      <c r="AH58" s="23"/>
+      <c r="AI58" s="23"/>
+      <c r="AJ58" s="23"/>
+      <c r="AK58" s="23"/>
+      <c r="AL58" s="23"/>
+      <c r="AM58" s="23"/>
+      <c r="AN58" s="23"/>
+      <c r="AO58" s="23"/>
+      <c r="AP58" s="23"/>
+      <c r="AQ58" s="23"/>
+      <c r="AR58" s="23"/>
+      <c r="AS58" s="23"/>
+      <c r="AT58" s="23"/>
     </row>
     <row r="59" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
-      <c r="J59" s="27"/>
-      <c r="K59" s="27"/>
-      <c r="L59" s="27"/>
-      <c r="M59" s="27"/>
-      <c r="N59" s="27"/>
-      <c r="O59" s="39"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="21"/>
+      <c r="N59" s="21"/>
+      <c r="O59" s="22"/>
       <c r="P59" s="15"/>
-      <c r="Q59" s="25"/>
-      <c r="R59" s="25"/>
-      <c r="S59" s="25"/>
-      <c r="T59" s="25"/>
-      <c r="U59" s="25"/>
-      <c r="V59" s="25"/>
-      <c r="W59" s="25"/>
-      <c r="X59" s="25"/>
-      <c r="Y59" s="25"/>
-      <c r="Z59" s="25"/>
-      <c r="AA59" s="25"/>
-      <c r="AB59" s="25"/>
-      <c r="AC59" s="25"/>
-      <c r="AD59" s="25"/>
-      <c r="AE59" s="25"/>
-      <c r="AF59" s="25"/>
-      <c r="AG59" s="25"/>
-      <c r="AH59" s="25"/>
-      <c r="AI59" s="25"/>
-      <c r="AJ59" s="25"/>
-      <c r="AK59" s="25"/>
-      <c r="AL59" s="25"/>
-      <c r="AM59" s="25"/>
-      <c r="AN59" s="25"/>
-      <c r="AO59" s="25"/>
-      <c r="AP59" s="25"/>
-      <c r="AQ59" s="25"/>
-      <c r="AR59" s="25"/>
-      <c r="AS59" s="25"/>
-      <c r="AT59" s="25"/>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="23"/>
+      <c r="S59" s="23"/>
+      <c r="T59" s="23"/>
+      <c r="U59" s="23"/>
+      <c r="V59" s="23"/>
+      <c r="W59" s="23"/>
+      <c r="X59" s="23"/>
+      <c r="Y59" s="23"/>
+      <c r="Z59" s="23"/>
+      <c r="AA59" s="23"/>
+      <c r="AB59" s="23"/>
+      <c r="AC59" s="23"/>
+      <c r="AD59" s="23"/>
+      <c r="AE59" s="23"/>
+      <c r="AF59" s="23"/>
+      <c r="AG59" s="23"/>
+      <c r="AH59" s="23"/>
+      <c r="AI59" s="23"/>
+      <c r="AJ59" s="23"/>
+      <c r="AK59" s="23"/>
+      <c r="AL59" s="23"/>
+      <c r="AM59" s="23"/>
+      <c r="AN59" s="23"/>
+      <c r="AO59" s="23"/>
+      <c r="AP59" s="23"/>
+      <c r="AQ59" s="23"/>
+      <c r="AR59" s="23"/>
+      <c r="AS59" s="23"/>
+      <c r="AT59" s="23"/>
     </row>
     <row r="60" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
-      <c r="K60" s="27"/>
-      <c r="L60" s="27"/>
-      <c r="M60" s="27"/>
-      <c r="N60" s="27"/>
-      <c r="O60" s="39"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="22"/>
       <c r="P60" s="15"/>
-      <c r="Q60" s="25"/>
-      <c r="R60" s="25"/>
-      <c r="S60" s="25"/>
-      <c r="T60" s="25"/>
-      <c r="U60" s="25"/>
-      <c r="V60" s="25"/>
-      <c r="W60" s="25"/>
-      <c r="X60" s="25"/>
-      <c r="Y60" s="25"/>
-      <c r="Z60" s="25"/>
-      <c r="AA60" s="25"/>
-      <c r="AB60" s="25"/>
-      <c r="AC60" s="25"/>
-      <c r="AD60" s="25"/>
-      <c r="AE60" s="25"/>
-      <c r="AF60" s="25"/>
-      <c r="AG60" s="25"/>
-      <c r="AH60" s="25"/>
-      <c r="AI60" s="25"/>
-      <c r="AJ60" s="25"/>
-      <c r="AK60" s="25"/>
-      <c r="AL60" s="25"/>
-      <c r="AM60" s="25"/>
-      <c r="AN60" s="25"/>
-      <c r="AO60" s="25"/>
-      <c r="AP60" s="25"/>
-      <c r="AQ60" s="25"/>
-      <c r="AR60" s="25"/>
-      <c r="AS60" s="25"/>
-      <c r="AT60" s="25"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="23"/>
+      <c r="S60" s="23"/>
+      <c r="T60" s="23"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="23"/>
+      <c r="W60" s="23"/>
+      <c r="X60" s="23"/>
+      <c r="Y60" s="23"/>
+      <c r="Z60" s="23"/>
+      <c r="AA60" s="23"/>
+      <c r="AB60" s="23"/>
+      <c r="AC60" s="23"/>
+      <c r="AD60" s="23"/>
+      <c r="AE60" s="23"/>
+      <c r="AF60" s="23"/>
+      <c r="AG60" s="23"/>
+      <c r="AH60" s="23"/>
+      <c r="AI60" s="23"/>
+      <c r="AJ60" s="23"/>
+      <c r="AK60" s="23"/>
+      <c r="AL60" s="23"/>
+      <c r="AM60" s="23"/>
+      <c r="AN60" s="23"/>
+      <c r="AO60" s="23"/>
+      <c r="AP60" s="23"/>
+      <c r="AQ60" s="23"/>
+      <c r="AR60" s="23"/>
+      <c r="AS60" s="23"/>
+      <c r="AT60" s="23"/>
     </row>
     <row r="61" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="27"/>
-      <c r="L61" s="27"/>
-      <c r="M61" s="27"/>
-      <c r="N61" s="27"/>
-      <c r="O61" s="39"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="22"/>
       <c r="P61" s="15"/>
-      <c r="Q61" s="25"/>
-      <c r="R61" s="25"/>
-      <c r="S61" s="25"/>
-      <c r="T61" s="25"/>
-      <c r="U61" s="25"/>
-      <c r="V61" s="25"/>
-      <c r="W61" s="25"/>
-      <c r="X61" s="25"/>
-      <c r="Y61" s="25"/>
-      <c r="Z61" s="25"/>
-      <c r="AA61" s="25"/>
-      <c r="AB61" s="25"/>
-      <c r="AC61" s="25"/>
-      <c r="AD61" s="25"/>
-      <c r="AE61" s="25"/>
-      <c r="AF61" s="25"/>
-      <c r="AG61" s="25"/>
-      <c r="AH61" s="25"/>
-      <c r="AI61" s="25"/>
-      <c r="AJ61" s="25"/>
-      <c r="AK61" s="25"/>
-      <c r="AL61" s="25"/>
-      <c r="AM61" s="25"/>
-      <c r="AN61" s="25"/>
-      <c r="AO61" s="25"/>
-      <c r="AP61" s="25"/>
-      <c r="AQ61" s="25"/>
-      <c r="AR61" s="25"/>
-      <c r="AS61" s="25"/>
-      <c r="AT61" s="25"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="23"/>
+      <c r="S61" s="23"/>
+      <c r="T61" s="23"/>
+      <c r="U61" s="23"/>
+      <c r="V61" s="23"/>
+      <c r="W61" s="23"/>
+      <c r="X61" s="23"/>
+      <c r="Y61" s="23"/>
+      <c r="Z61" s="23"/>
+      <c r="AA61" s="23"/>
+      <c r="AB61" s="23"/>
+      <c r="AC61" s="23"/>
+      <c r="AD61" s="23"/>
+      <c r="AE61" s="23"/>
+      <c r="AF61" s="23"/>
+      <c r="AG61" s="23"/>
+      <c r="AH61" s="23"/>
+      <c r="AI61" s="23"/>
+      <c r="AJ61" s="23"/>
+      <c r="AK61" s="23"/>
+      <c r="AL61" s="23"/>
+      <c r="AM61" s="23"/>
+      <c r="AN61" s="23"/>
+      <c r="AO61" s="23"/>
+      <c r="AP61" s="23"/>
+      <c r="AQ61" s="23"/>
+      <c r="AR61" s="23"/>
+      <c r="AS61" s="23"/>
+      <c r="AT61" s="23"/>
     </row>
     <row r="62" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="27"/>
-      <c r="N62" s="27"/>
-      <c r="O62" s="39"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="21"/>
+      <c r="O62" s="22"/>
       <c r="P62" s="15"/>
-      <c r="Q62" s="25"/>
-      <c r="R62" s="25"/>
-      <c r="S62" s="25"/>
-      <c r="T62" s="25"/>
-      <c r="U62" s="25"/>
-      <c r="V62" s="25"/>
-      <c r="W62" s="25"/>
-      <c r="X62" s="25"/>
-      <c r="Y62" s="25"/>
-      <c r="Z62" s="25"/>
-      <c r="AA62" s="25"/>
-      <c r="AB62" s="25"/>
-      <c r="AC62" s="25"/>
-      <c r="AD62" s="25"/>
-      <c r="AE62" s="25"/>
-      <c r="AF62" s="25"/>
-      <c r="AG62" s="25"/>
-      <c r="AH62" s="25"/>
-      <c r="AI62" s="25"/>
-      <c r="AJ62" s="25"/>
-      <c r="AK62" s="25"/>
-      <c r="AL62" s="25"/>
-      <c r="AM62" s="25"/>
-      <c r="AN62" s="25"/>
-      <c r="AO62" s="25"/>
-      <c r="AP62" s="25"/>
-      <c r="AQ62" s="25"/>
-      <c r="AR62" s="25"/>
-      <c r="AS62" s="25"/>
-      <c r="AT62" s="25"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="23"/>
+      <c r="S62" s="23"/>
+      <c r="T62" s="23"/>
+      <c r="U62" s="23"/>
+      <c r="V62" s="23"/>
+      <c r="W62" s="23"/>
+      <c r="X62" s="23"/>
+      <c r="Y62" s="23"/>
+      <c r="Z62" s="23"/>
+      <c r="AA62" s="23"/>
+      <c r="AB62" s="23"/>
+      <c r="AC62" s="23"/>
+      <c r="AD62" s="23"/>
+      <c r="AE62" s="23"/>
+      <c r="AF62" s="23"/>
+      <c r="AG62" s="23"/>
+      <c r="AH62" s="23"/>
+      <c r="AI62" s="23"/>
+      <c r="AJ62" s="23"/>
+      <c r="AK62" s="23"/>
+      <c r="AL62" s="23"/>
+      <c r="AM62" s="23"/>
+      <c r="AN62" s="23"/>
+      <c r="AO62" s="23"/>
+      <c r="AP62" s="23"/>
+      <c r="AQ62" s="23"/>
+      <c r="AR62" s="23"/>
+      <c r="AS62" s="23"/>
+      <c r="AT62" s="23"/>
     </row>
     <row r="63" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
-      <c r="J63" s="27"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="27"/>
-      <c r="M63" s="27"/>
-      <c r="N63" s="27"/>
-      <c r="O63" s="39"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="21"/>
+      <c r="N63" s="21"/>
+      <c r="O63" s="22"/>
       <c r="P63" s="15"/>
-      <c r="Q63" s="25"/>
-      <c r="R63" s="25"/>
-      <c r="S63" s="25"/>
-      <c r="T63" s="25"/>
-      <c r="U63" s="25"/>
-      <c r="V63" s="25"/>
-      <c r="W63" s="25"/>
-      <c r="X63" s="25"/>
-      <c r="Y63" s="25"/>
-      <c r="Z63" s="25"/>
-      <c r="AA63" s="25"/>
-      <c r="AB63" s="25"/>
-      <c r="AC63" s="25"/>
-      <c r="AD63" s="25"/>
-      <c r="AE63" s="25"/>
-      <c r="AF63" s="25"/>
-      <c r="AG63" s="25"/>
-      <c r="AH63" s="25"/>
-      <c r="AI63" s="25"/>
-      <c r="AJ63" s="25"/>
-      <c r="AK63" s="25"/>
-      <c r="AL63" s="25"/>
-      <c r="AM63" s="25"/>
-      <c r="AN63" s="25"/>
-      <c r="AO63" s="25"/>
-      <c r="AP63" s="25"/>
-      <c r="AQ63" s="25"/>
-      <c r="AR63" s="25"/>
-      <c r="AS63" s="25"/>
-      <c r="AT63" s="25"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="23"/>
+      <c r="S63" s="23"/>
+      <c r="T63" s="23"/>
+      <c r="U63" s="23"/>
+      <c r="V63" s="23"/>
+      <c r="W63" s="23"/>
+      <c r="X63" s="23"/>
+      <c r="Y63" s="23"/>
+      <c r="Z63" s="23"/>
+      <c r="AA63" s="23"/>
+      <c r="AB63" s="23"/>
+      <c r="AC63" s="23"/>
+      <c r="AD63" s="23"/>
+      <c r="AE63" s="23"/>
+      <c r="AF63" s="23"/>
+      <c r="AG63" s="23"/>
+      <c r="AH63" s="23"/>
+      <c r="AI63" s="23"/>
+      <c r="AJ63" s="23"/>
+      <c r="AK63" s="23"/>
+      <c r="AL63" s="23"/>
+      <c r="AM63" s="23"/>
+      <c r="AN63" s="23"/>
+      <c r="AO63" s="23"/>
+      <c r="AP63" s="23"/>
+      <c r="AQ63" s="23"/>
+      <c r="AR63" s="23"/>
+      <c r="AS63" s="23"/>
+      <c r="AT63" s="23"/>
     </row>
     <row r="64" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="27"/>
-      <c r="M64" s="27"/>
-      <c r="N64" s="27"/>
-      <c r="O64" s="39"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="21"/>
+      <c r="N64" s="21"/>
+      <c r="O64" s="22"/>
       <c r="P64" s="15"/>
-      <c r="Q64" s="25"/>
-      <c r="R64" s="25"/>
-      <c r="S64" s="25"/>
-      <c r="T64" s="25"/>
-      <c r="U64" s="25"/>
-      <c r="V64" s="25"/>
-      <c r="W64" s="25"/>
-      <c r="X64" s="25"/>
-      <c r="Y64" s="25"/>
-      <c r="Z64" s="25"/>
-      <c r="AA64" s="25"/>
-      <c r="AB64" s="25"/>
-      <c r="AC64" s="25"/>
-      <c r="AD64" s="25"/>
-      <c r="AE64" s="25"/>
-      <c r="AF64" s="25"/>
-      <c r="AG64" s="25"/>
-      <c r="AH64" s="25"/>
-      <c r="AI64" s="25"/>
-      <c r="AJ64" s="25"/>
-      <c r="AK64" s="25"/>
-      <c r="AL64" s="25"/>
-      <c r="AM64" s="25"/>
-      <c r="AN64" s="25"/>
-      <c r="AO64" s="25"/>
-      <c r="AP64" s="25"/>
-      <c r="AQ64" s="25"/>
-      <c r="AR64" s="25"/>
-      <c r="AS64" s="25"/>
-      <c r="AT64" s="25"/>
+      <c r="Q64" s="23"/>
+      <c r="R64" s="23"/>
+      <c r="S64" s="23"/>
+      <c r="T64" s="23"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="23"/>
+      <c r="W64" s="23"/>
+      <c r="X64" s="23"/>
+      <c r="Y64" s="23"/>
+      <c r="Z64" s="23"/>
+      <c r="AA64" s="23"/>
+      <c r="AB64" s="23"/>
+      <c r="AC64" s="23"/>
+      <c r="AD64" s="23"/>
+      <c r="AE64" s="23"/>
+      <c r="AF64" s="23"/>
+      <c r="AG64" s="23"/>
+      <c r="AH64" s="23"/>
+      <c r="AI64" s="23"/>
+      <c r="AJ64" s="23"/>
+      <c r="AK64" s="23"/>
+      <c r="AL64" s="23"/>
+      <c r="AM64" s="23"/>
+      <c r="AN64" s="23"/>
+      <c r="AO64" s="23"/>
+      <c r="AP64" s="23"/>
+      <c r="AQ64" s="23"/>
+      <c r="AR64" s="23"/>
+      <c r="AS64" s="23"/>
+      <c r="AT64" s="23"/>
     </row>
     <row r="65" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
-      <c r="J65" s="27"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
-      <c r="N65" s="27"/>
-      <c r="O65" s="39"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="21"/>
+      <c r="N65" s="21"/>
+      <c r="O65" s="22"/>
       <c r="P65" s="15"/>
-      <c r="Q65" s="25"/>
-      <c r="R65" s="25"/>
-      <c r="S65" s="25"/>
-      <c r="T65" s="25"/>
-      <c r="U65" s="25"/>
-      <c r="V65" s="25"/>
-      <c r="W65" s="25"/>
-      <c r="X65" s="25"/>
-      <c r="Y65" s="25"/>
-      <c r="Z65" s="25"/>
-      <c r="AA65" s="25"/>
-      <c r="AB65" s="25"/>
-      <c r="AC65" s="25"/>
-      <c r="AD65" s="25"/>
-      <c r="AE65" s="25"/>
-      <c r="AF65" s="25"/>
-      <c r="AG65" s="25"/>
-      <c r="AH65" s="25"/>
-      <c r="AI65" s="25"/>
-      <c r="AJ65" s="25"/>
-      <c r="AK65" s="25"/>
-      <c r="AL65" s="25"/>
-      <c r="AM65" s="25"/>
-      <c r="AN65" s="25"/>
-      <c r="AO65" s="25"/>
-      <c r="AP65" s="25"/>
-      <c r="AQ65" s="25"/>
-      <c r="AR65" s="25"/>
-      <c r="AS65" s="25"/>
-      <c r="AT65" s="25"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="23"/>
+      <c r="S65" s="23"/>
+      <c r="T65" s="23"/>
+      <c r="U65" s="23"/>
+      <c r="V65" s="23"/>
+      <c r="W65" s="23"/>
+      <c r="X65" s="23"/>
+      <c r="Y65" s="23"/>
+      <c r="Z65" s="23"/>
+      <c r="AA65" s="23"/>
+      <c r="AB65" s="23"/>
+      <c r="AC65" s="23"/>
+      <c r="AD65" s="23"/>
+      <c r="AE65" s="23"/>
+      <c r="AF65" s="23"/>
+      <c r="AG65" s="23"/>
+      <c r="AH65" s="23"/>
+      <c r="AI65" s="23"/>
+      <c r="AJ65" s="23"/>
+      <c r="AK65" s="23"/>
+      <c r="AL65" s="23"/>
+      <c r="AM65" s="23"/>
+      <c r="AN65" s="23"/>
+      <c r="AO65" s="23"/>
+      <c r="AP65" s="23"/>
+      <c r="AQ65" s="23"/>
+      <c r="AR65" s="23"/>
+      <c r="AS65" s="23"/>
+      <c r="AT65" s="23"/>
     </row>
     <row r="66" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
-      <c r="J66" s="27"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="27"/>
-      <c r="N66" s="27"/>
-      <c r="O66" s="39"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+      <c r="N66" s="21"/>
+      <c r="O66" s="22"/>
       <c r="P66" s="15"/>
-      <c r="Q66" s="25"/>
-      <c r="R66" s="25"/>
-      <c r="S66" s="25"/>
-      <c r="T66" s="25"/>
-      <c r="U66" s="25"/>
-      <c r="V66" s="25"/>
-      <c r="W66" s="25"/>
-      <c r="X66" s="25"/>
-      <c r="Y66" s="25"/>
-      <c r="Z66" s="25"/>
-      <c r="AA66" s="25"/>
-      <c r="AB66" s="25"/>
-      <c r="AC66" s="25"/>
-      <c r="AD66" s="25"/>
-      <c r="AE66" s="25"/>
-      <c r="AF66" s="25"/>
-      <c r="AG66" s="25"/>
-      <c r="AH66" s="25"/>
-      <c r="AI66" s="25"/>
-      <c r="AJ66" s="25"/>
-      <c r="AK66" s="25"/>
-      <c r="AL66" s="25"/>
-      <c r="AM66" s="25"/>
-      <c r="AN66" s="25"/>
-      <c r="AO66" s="25"/>
-      <c r="AP66" s="25"/>
-      <c r="AQ66" s="25"/>
-      <c r="AR66" s="25"/>
-      <c r="AS66" s="25"/>
-      <c r="AT66" s="25"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="23"/>
+      <c r="S66" s="23"/>
+      <c r="T66" s="23"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="23"/>
+      <c r="W66" s="23"/>
+      <c r="X66" s="23"/>
+      <c r="Y66" s="23"/>
+      <c r="Z66" s="23"/>
+      <c r="AA66" s="23"/>
+      <c r="AB66" s="23"/>
+      <c r="AC66" s="23"/>
+      <c r="AD66" s="23"/>
+      <c r="AE66" s="23"/>
+      <c r="AF66" s="23"/>
+      <c r="AG66" s="23"/>
+      <c r="AH66" s="23"/>
+      <c r="AI66" s="23"/>
+      <c r="AJ66" s="23"/>
+      <c r="AK66" s="23"/>
+      <c r="AL66" s="23"/>
+      <c r="AM66" s="23"/>
+      <c r="AN66" s="23"/>
+      <c r="AO66" s="23"/>
+      <c r="AP66" s="23"/>
+      <c r="AQ66" s="23"/>
+      <c r="AR66" s="23"/>
+      <c r="AS66" s="23"/>
+      <c r="AT66" s="23"/>
     </row>
     <row r="67" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-      <c r="O67" s="39"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="21"/>
+      <c r="N67" s="21"/>
+      <c r="O67" s="22"/>
       <c r="P67" s="15"/>
-      <c r="Q67" s="25"/>
-      <c r="R67" s="25"/>
-      <c r="S67" s="25"/>
-      <c r="T67" s="25"/>
-      <c r="U67" s="25"/>
-      <c r="V67" s="25"/>
-      <c r="W67" s="25"/>
-      <c r="X67" s="25"/>
-      <c r="Y67" s="25"/>
-      <c r="Z67" s="25"/>
-      <c r="AA67" s="25"/>
-      <c r="AB67" s="25"/>
-      <c r="AC67" s="25"/>
-      <c r="AD67" s="25"/>
-      <c r="AE67" s="25"/>
-      <c r="AF67" s="25"/>
-      <c r="AG67" s="25"/>
-      <c r="AH67" s="25"/>
-      <c r="AI67" s="25"/>
-      <c r="AJ67" s="25"/>
-      <c r="AK67" s="25"/>
-      <c r="AL67" s="25"/>
-      <c r="AM67" s="25"/>
-      <c r="AN67" s="25"/>
-      <c r="AO67" s="25"/>
-      <c r="AP67" s="25"/>
-      <c r="AQ67" s="25"/>
-      <c r="AR67" s="25"/>
-      <c r="AS67" s="25"/>
-      <c r="AT67" s="25"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="23"/>
+      <c r="S67" s="23"/>
+      <c r="T67" s="23"/>
+      <c r="U67" s="23"/>
+      <c r="V67" s="23"/>
+      <c r="W67" s="23"/>
+      <c r="X67" s="23"/>
+      <c r="Y67" s="23"/>
+      <c r="Z67" s="23"/>
+      <c r="AA67" s="23"/>
+      <c r="AB67" s="23"/>
+      <c r="AC67" s="23"/>
+      <c r="AD67" s="23"/>
+      <c r="AE67" s="23"/>
+      <c r="AF67" s="23"/>
+      <c r="AG67" s="23"/>
+      <c r="AH67" s="23"/>
+      <c r="AI67" s="23"/>
+      <c r="AJ67" s="23"/>
+      <c r="AK67" s="23"/>
+      <c r="AL67" s="23"/>
+      <c r="AM67" s="23"/>
+      <c r="AN67" s="23"/>
+      <c r="AO67" s="23"/>
+      <c r="AP67" s="23"/>
+      <c r="AQ67" s="23"/>
+      <c r="AR67" s="23"/>
+      <c r="AS67" s="23"/>
+      <c r="AT67" s="23"/>
     </row>
     <row r="68" spans="1:46" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="27"/>
-      <c r="I68" s="27"/>
-      <c r="J68" s="27"/>
-      <c r="K68" s="27"/>
-      <c r="L68" s="27"/>
-      <c r="M68" s="27"/>
-      <c r="N68" s="27"/>
-      <c r="O68" s="39"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="21"/>
+      <c r="N68" s="21"/>
+      <c r="O68" s="22"/>
       <c r="P68" s="15"/>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25"/>
-      <c r="S68" s="25"/>
-      <c r="T68" s="25"/>
-      <c r="U68" s="25"/>
-      <c r="V68" s="25"/>
-      <c r="W68" s="25"/>
-      <c r="X68" s="25"/>
-      <c r="Y68" s="25"/>
-      <c r="Z68" s="25"/>
-      <c r="AA68" s="25"/>
-      <c r="AB68" s="25"/>
-      <c r="AC68" s="25"/>
-      <c r="AD68" s="25"/>
-      <c r="AE68" s="25"/>
-      <c r="AF68" s="25"/>
-      <c r="AG68" s="25"/>
-      <c r="AH68" s="25"/>
-      <c r="AI68" s="25"/>
-      <c r="AJ68" s="25"/>
-      <c r="AK68" s="25"/>
-      <c r="AL68" s="25"/>
-      <c r="AM68" s="25"/>
-      <c r="AN68" s="25"/>
-      <c r="AO68" s="25"/>
-      <c r="AP68" s="25"/>
-      <c r="AQ68" s="25"/>
-      <c r="AR68" s="25"/>
-      <c r="AS68" s="25"/>
-      <c r="AT68" s="25"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="23"/>
+      <c r="S68" s="23"/>
+      <c r="T68" s="23"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="23"/>
+      <c r="W68" s="23"/>
+      <c r="X68" s="23"/>
+      <c r="Y68" s="23"/>
+      <c r="Z68" s="23"/>
+      <c r="AA68" s="23"/>
+      <c r="AB68" s="23"/>
+      <c r="AC68" s="23"/>
+      <c r="AD68" s="23"/>
+      <c r="AE68" s="23"/>
+      <c r="AF68" s="23"/>
+      <c r="AG68" s="23"/>
+      <c r="AH68" s="23"/>
+      <c r="AI68" s="23"/>
+      <c r="AJ68" s="23"/>
+      <c r="AK68" s="23"/>
+      <c r="AL68" s="23"/>
+      <c r="AM68" s="23"/>
+      <c r="AN68" s="23"/>
+      <c r="AO68" s="23"/>
+      <c r="AP68" s="23"/>
+      <c r="AQ68" s="23"/>
+      <c r="AR68" s="23"/>
+      <c r="AS68" s="23"/>
+      <c r="AT68" s="23"/>
     </row>
     <row r="69" spans="1:46" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
@@ -4044,7 +4088,7 @@
       <c r="AQ70" s="12"/>
       <c r="AR70" s="12"/>
       <c r="AS70" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AT70" s="12"/>
     </row>
@@ -4094,7 +4138,7 @@
       <c r="AQ71" s="12"/>
       <c r="AR71" s="12"/>
       <c r="AS71" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AT71" s="12"/>
     </row>
@@ -9193,159 +9237,64 @@
     <row r="182" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="235">
-    <mergeCell ref="C60:O60"/>
-    <mergeCell ref="Q60:S60"/>
-    <mergeCell ref="C61:O61"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="C62:O62"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="C63:O63"/>
-    <mergeCell ref="Q63:S63"/>
-    <mergeCell ref="C64:O64"/>
-    <mergeCell ref="Q64:S64"/>
-    <mergeCell ref="C47:O47"/>
-    <mergeCell ref="Q47:S47"/>
-    <mergeCell ref="C48:O48"/>
-    <mergeCell ref="Q48:S48"/>
-    <mergeCell ref="C49:O49"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="C50:O50"/>
-    <mergeCell ref="Q50:S50"/>
-    <mergeCell ref="C51:O51"/>
-    <mergeCell ref="Q51:S51"/>
-    <mergeCell ref="T68:Z68"/>
-    <mergeCell ref="AA68:AG68"/>
-    <mergeCell ref="AH68:AM68"/>
-    <mergeCell ref="AN68:AT68"/>
-    <mergeCell ref="T67:Z67"/>
-    <mergeCell ref="AA67:AG67"/>
-    <mergeCell ref="AH67:AM67"/>
-    <mergeCell ref="AN67:AT67"/>
-    <mergeCell ref="C67:O67"/>
-    <mergeCell ref="Q67:S67"/>
-    <mergeCell ref="C68:O68"/>
-    <mergeCell ref="Q68:S68"/>
-    <mergeCell ref="T66:Z66"/>
-    <mergeCell ref="AA66:AG66"/>
-    <mergeCell ref="AH66:AM66"/>
-    <mergeCell ref="AN66:AT66"/>
-    <mergeCell ref="T65:Z65"/>
-    <mergeCell ref="AA65:AG65"/>
-    <mergeCell ref="AH65:AM65"/>
-    <mergeCell ref="AN65:AT65"/>
-    <mergeCell ref="C65:O65"/>
-    <mergeCell ref="Q65:S65"/>
-    <mergeCell ref="C66:O66"/>
-    <mergeCell ref="Q66:S66"/>
-    <mergeCell ref="AH61:AM61"/>
-    <mergeCell ref="AN61:AT61"/>
-    <mergeCell ref="T64:Z64"/>
-    <mergeCell ref="AA64:AG64"/>
-    <mergeCell ref="AH64:AM64"/>
-    <mergeCell ref="AN64:AT64"/>
-    <mergeCell ref="T63:Z63"/>
-    <mergeCell ref="AA63:AG63"/>
-    <mergeCell ref="AH63:AM63"/>
-    <mergeCell ref="AN63:AT63"/>
-    <mergeCell ref="AN57:AT57"/>
-    <mergeCell ref="T56:Z56"/>
-    <mergeCell ref="AA56:AG56"/>
-    <mergeCell ref="AH56:AM56"/>
-    <mergeCell ref="AN56:AT56"/>
-    <mergeCell ref="C56:O56"/>
-    <mergeCell ref="Q56:S56"/>
-    <mergeCell ref="C57:O57"/>
-    <mergeCell ref="Q57:S57"/>
-    <mergeCell ref="AN55:AT55"/>
-    <mergeCell ref="T54:Z54"/>
-    <mergeCell ref="AA54:AG54"/>
-    <mergeCell ref="AH54:AM54"/>
-    <mergeCell ref="AN54:AT54"/>
-    <mergeCell ref="C54:O54"/>
-    <mergeCell ref="Q54:S54"/>
-    <mergeCell ref="C55:O55"/>
-    <mergeCell ref="Q55:S55"/>
-    <mergeCell ref="AN53:AT53"/>
-    <mergeCell ref="T52:Z52"/>
-    <mergeCell ref="AA52:AG52"/>
-    <mergeCell ref="AH52:AM52"/>
-    <mergeCell ref="AN52:AT52"/>
-    <mergeCell ref="C52:O52"/>
-    <mergeCell ref="Q52:S52"/>
-    <mergeCell ref="C53:O53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="AN48:AT48"/>
-    <mergeCell ref="T51:Z51"/>
-    <mergeCell ref="AA51:AG51"/>
-    <mergeCell ref="AH51:AM51"/>
-    <mergeCell ref="AN51:AT51"/>
-    <mergeCell ref="T50:Z50"/>
-    <mergeCell ref="AA50:AG50"/>
-    <mergeCell ref="AH50:AM50"/>
-    <mergeCell ref="AN50:AT50"/>
-    <mergeCell ref="AN42:AT42"/>
-    <mergeCell ref="T41:Z41"/>
-    <mergeCell ref="AA41:AG41"/>
-    <mergeCell ref="AH41:AM41"/>
-    <mergeCell ref="AN41:AT41"/>
-    <mergeCell ref="C42:O42"/>
-    <mergeCell ref="Q42:S42"/>
-    <mergeCell ref="T44:Z44"/>
-    <mergeCell ref="AA44:AG44"/>
-    <mergeCell ref="AH44:AM44"/>
-    <mergeCell ref="AN44:AT44"/>
-    <mergeCell ref="T43:Z43"/>
-    <mergeCell ref="AA43:AG43"/>
-    <mergeCell ref="AH43:AM43"/>
-    <mergeCell ref="AN43:AT43"/>
-    <mergeCell ref="C43:O43"/>
-    <mergeCell ref="Q43:S43"/>
-    <mergeCell ref="C44:O44"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="C41:O41"/>
-    <mergeCell ref="Q41:S41"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A34:B37"/>
-    <mergeCell ref="C34:O37"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="P34:P37"/>
-    <mergeCell ref="T42:Z42"/>
-    <mergeCell ref="AA42:AG42"/>
-    <mergeCell ref="AH42:AM42"/>
-    <mergeCell ref="Q34:S37"/>
-    <mergeCell ref="C38:O38"/>
-    <mergeCell ref="Q38:S38"/>
-    <mergeCell ref="C39:O39"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="C40:O40"/>
-    <mergeCell ref="Q40:S40"/>
-    <mergeCell ref="T40:Z40"/>
-    <mergeCell ref="AA40:AG40"/>
-    <mergeCell ref="AH40:AM40"/>
-    <mergeCell ref="AN40:AT40"/>
-    <mergeCell ref="AN34:AT37"/>
-    <mergeCell ref="AH34:AM37"/>
-    <mergeCell ref="AA34:AG37"/>
-    <mergeCell ref="T34:Z37"/>
-    <mergeCell ref="T38:Z38"/>
-    <mergeCell ref="AA38:AG38"/>
-    <mergeCell ref="AH38:AM38"/>
-    <mergeCell ref="AN38:AT38"/>
-    <mergeCell ref="T39:Z39"/>
-    <mergeCell ref="AA39:AG39"/>
-    <mergeCell ref="AH39:AM39"/>
-    <mergeCell ref="AN39:AT39"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C45:O45"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="C46:O46"/>
-    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="M21:AT21"/>
+    <mergeCell ref="A1:AT1"/>
+    <mergeCell ref="A3:AT3"/>
+    <mergeCell ref="A2:AT2"/>
+    <mergeCell ref="A4:AT4"/>
+    <mergeCell ref="A11:AT11"/>
+    <mergeCell ref="A12:AT12"/>
+    <mergeCell ref="M16:AT16"/>
+    <mergeCell ref="M17:AT17"/>
+    <mergeCell ref="M20:AT20"/>
+    <mergeCell ref="AN58:AT58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="T60:Z60"/>
+    <mergeCell ref="AA60:AG60"/>
+    <mergeCell ref="AH60:AM60"/>
+    <mergeCell ref="AN60:AT60"/>
+    <mergeCell ref="T59:Z59"/>
+    <mergeCell ref="AA59:AG59"/>
+    <mergeCell ref="AH59:AM59"/>
+    <mergeCell ref="AN59:AT59"/>
+    <mergeCell ref="T62:Z62"/>
+    <mergeCell ref="Q58:S58"/>
+    <mergeCell ref="C59:O59"/>
+    <mergeCell ref="Q59:S59"/>
+    <mergeCell ref="AA62:AG62"/>
+    <mergeCell ref="AH62:AM62"/>
+    <mergeCell ref="AN62:AT62"/>
+    <mergeCell ref="T61:Z61"/>
+    <mergeCell ref="AA61:AG61"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="T58:Z58"/>
+    <mergeCell ref="AA58:AG58"/>
+    <mergeCell ref="AH58:AM58"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:O58"/>
+    <mergeCell ref="T53:Z53"/>
+    <mergeCell ref="AA53:AG53"/>
+    <mergeCell ref="AH53:AM53"/>
+    <mergeCell ref="T55:Z55"/>
+    <mergeCell ref="AA55:AG55"/>
+    <mergeCell ref="AH55:AM55"/>
+    <mergeCell ref="T57:Z57"/>
+    <mergeCell ref="AA57:AG57"/>
+    <mergeCell ref="AH57:AM57"/>
     <mergeCell ref="T45:Z45"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A50:B50"/>
@@ -9370,64 +9319,159 @@
     <mergeCell ref="T48:Z48"/>
     <mergeCell ref="AA48:AG48"/>
     <mergeCell ref="AH48:AM48"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="T58:Z58"/>
-    <mergeCell ref="AA58:AG58"/>
-    <mergeCell ref="AH58:AM58"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:O58"/>
-    <mergeCell ref="T53:Z53"/>
-    <mergeCell ref="AA53:AG53"/>
-    <mergeCell ref="AH53:AM53"/>
-    <mergeCell ref="T55:Z55"/>
-    <mergeCell ref="AA55:AG55"/>
-    <mergeCell ref="AH55:AM55"/>
-    <mergeCell ref="T57:Z57"/>
-    <mergeCell ref="AA57:AG57"/>
-    <mergeCell ref="AH57:AM57"/>
-    <mergeCell ref="AN58:AT58"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="T60:Z60"/>
-    <mergeCell ref="AA60:AG60"/>
-    <mergeCell ref="AH60:AM60"/>
-    <mergeCell ref="AN60:AT60"/>
-    <mergeCell ref="T59:Z59"/>
-    <mergeCell ref="AA59:AG59"/>
-    <mergeCell ref="AH59:AM59"/>
-    <mergeCell ref="AN59:AT59"/>
-    <mergeCell ref="T62:Z62"/>
-    <mergeCell ref="Q58:S58"/>
-    <mergeCell ref="C59:O59"/>
-    <mergeCell ref="Q59:S59"/>
-    <mergeCell ref="AA62:AG62"/>
-    <mergeCell ref="AH62:AM62"/>
-    <mergeCell ref="AN62:AT62"/>
-    <mergeCell ref="T61:Z61"/>
-    <mergeCell ref="AA61:AG61"/>
-    <mergeCell ref="M21:AT21"/>
-    <mergeCell ref="A1:AT1"/>
-    <mergeCell ref="A3:AT3"/>
-    <mergeCell ref="A2:AT2"/>
-    <mergeCell ref="A4:AT4"/>
-    <mergeCell ref="A11:AT11"/>
-    <mergeCell ref="A12:AT12"/>
-    <mergeCell ref="M16:AT16"/>
-    <mergeCell ref="M17:AT17"/>
-    <mergeCell ref="M20:AT20"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C45:O45"/>
+    <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="C46:O46"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="AN40:AT40"/>
+    <mergeCell ref="AN34:AT37"/>
+    <mergeCell ref="AH34:AM37"/>
+    <mergeCell ref="AA34:AG37"/>
+    <mergeCell ref="T34:Z37"/>
+    <mergeCell ref="T38:Z38"/>
+    <mergeCell ref="AA38:AG38"/>
+    <mergeCell ref="AH38:AM38"/>
+    <mergeCell ref="AN38:AT38"/>
+    <mergeCell ref="T39:Z39"/>
+    <mergeCell ref="AA39:AG39"/>
+    <mergeCell ref="AH39:AM39"/>
+    <mergeCell ref="AN39:AT39"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A34:B37"/>
+    <mergeCell ref="C34:O37"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="P34:P37"/>
+    <mergeCell ref="T42:Z42"/>
+    <mergeCell ref="AA42:AG42"/>
+    <mergeCell ref="AH42:AM42"/>
+    <mergeCell ref="Q34:S37"/>
+    <mergeCell ref="C38:O38"/>
+    <mergeCell ref="Q38:S38"/>
+    <mergeCell ref="C39:O39"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="C40:O40"/>
+    <mergeCell ref="Q40:S40"/>
+    <mergeCell ref="T40:Z40"/>
+    <mergeCell ref="AA40:AG40"/>
+    <mergeCell ref="AH40:AM40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="AN42:AT42"/>
+    <mergeCell ref="T41:Z41"/>
+    <mergeCell ref="AA41:AG41"/>
+    <mergeCell ref="AH41:AM41"/>
+    <mergeCell ref="AN41:AT41"/>
+    <mergeCell ref="C42:O42"/>
+    <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="T44:Z44"/>
+    <mergeCell ref="AA44:AG44"/>
+    <mergeCell ref="AH44:AM44"/>
+    <mergeCell ref="AN44:AT44"/>
+    <mergeCell ref="T43:Z43"/>
+    <mergeCell ref="AA43:AG43"/>
+    <mergeCell ref="AH43:AM43"/>
+    <mergeCell ref="AN43:AT43"/>
+    <mergeCell ref="C43:O43"/>
+    <mergeCell ref="Q43:S43"/>
+    <mergeCell ref="C44:O44"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="C41:O41"/>
+    <mergeCell ref="Q41:S41"/>
+    <mergeCell ref="AN48:AT48"/>
+    <mergeCell ref="T51:Z51"/>
+    <mergeCell ref="AA51:AG51"/>
+    <mergeCell ref="AH51:AM51"/>
+    <mergeCell ref="AN51:AT51"/>
+    <mergeCell ref="T50:Z50"/>
+    <mergeCell ref="AA50:AG50"/>
+    <mergeCell ref="AH50:AM50"/>
+    <mergeCell ref="AN50:AT50"/>
+    <mergeCell ref="AN53:AT53"/>
+    <mergeCell ref="T52:Z52"/>
+    <mergeCell ref="AA52:AG52"/>
+    <mergeCell ref="AH52:AM52"/>
+    <mergeCell ref="AN52:AT52"/>
+    <mergeCell ref="C52:O52"/>
+    <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="C53:O53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="AN55:AT55"/>
+    <mergeCell ref="T54:Z54"/>
+    <mergeCell ref="AA54:AG54"/>
+    <mergeCell ref="AH54:AM54"/>
+    <mergeCell ref="AN54:AT54"/>
+    <mergeCell ref="C54:O54"/>
+    <mergeCell ref="Q54:S54"/>
+    <mergeCell ref="C55:O55"/>
+    <mergeCell ref="Q55:S55"/>
+    <mergeCell ref="AN57:AT57"/>
+    <mergeCell ref="T56:Z56"/>
+    <mergeCell ref="AA56:AG56"/>
+    <mergeCell ref="AH56:AM56"/>
+    <mergeCell ref="AN56:AT56"/>
+    <mergeCell ref="C56:O56"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="C57:O57"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="AH61:AM61"/>
+    <mergeCell ref="AN61:AT61"/>
+    <mergeCell ref="T64:Z64"/>
+    <mergeCell ref="AA64:AG64"/>
+    <mergeCell ref="AH64:AM64"/>
+    <mergeCell ref="AN64:AT64"/>
+    <mergeCell ref="T63:Z63"/>
+    <mergeCell ref="AA63:AG63"/>
+    <mergeCell ref="AH63:AM63"/>
+    <mergeCell ref="AN63:AT63"/>
+    <mergeCell ref="T66:Z66"/>
+    <mergeCell ref="AA66:AG66"/>
+    <mergeCell ref="AH66:AM66"/>
+    <mergeCell ref="AN66:AT66"/>
+    <mergeCell ref="T65:Z65"/>
+    <mergeCell ref="AA65:AG65"/>
+    <mergeCell ref="AH65:AM65"/>
+    <mergeCell ref="AN65:AT65"/>
+    <mergeCell ref="C65:O65"/>
+    <mergeCell ref="Q65:S65"/>
+    <mergeCell ref="C66:O66"/>
+    <mergeCell ref="Q66:S66"/>
+    <mergeCell ref="T68:Z68"/>
+    <mergeCell ref="AA68:AG68"/>
+    <mergeCell ref="AH68:AM68"/>
+    <mergeCell ref="AN68:AT68"/>
+    <mergeCell ref="T67:Z67"/>
+    <mergeCell ref="AA67:AG67"/>
+    <mergeCell ref="AH67:AM67"/>
+    <mergeCell ref="AN67:AT67"/>
+    <mergeCell ref="C67:O67"/>
+    <mergeCell ref="Q67:S67"/>
+    <mergeCell ref="C68:O68"/>
+    <mergeCell ref="Q68:S68"/>
+    <mergeCell ref="C47:O47"/>
+    <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="C48:O48"/>
+    <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="C49:O49"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="C50:O50"/>
+    <mergeCell ref="Q50:S50"/>
+    <mergeCell ref="C51:O51"/>
+    <mergeCell ref="Q51:S51"/>
+    <mergeCell ref="C60:O60"/>
+    <mergeCell ref="Q60:S60"/>
+    <mergeCell ref="C61:O61"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="C62:O62"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="C63:O63"/>
+    <mergeCell ref="Q63:S63"/>
+    <mergeCell ref="C64:O64"/>
+    <mergeCell ref="Q64:S64"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -9435,7 +9479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>